<commit_message>
added primeiro de maio
</commit_message>
<xml_diff>
--- a/data/dados.xlsx
+++ b/data/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\reajuste\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0870539-0E7E-4346-A648-E02BE67CBEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B96A45-F7AA-4F89-B35C-35C72B9207A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{BE2A1F3B-6535-41F1-9783-CEB15E5262F6}"/>
+    <workbookView xWindow="21795" yWindow="3615" windowWidth="15765" windowHeight="11295" xr2:uid="{BE2A1F3B-6535-41F1-9783-CEB15E5262F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="53">
   <si>
     <t>Cafeara</t>
   </si>
   <si>
-    <t>Centenario do Sul</t>
-  </si>
-  <si>
-    <t>Lupionopolis</t>
-  </si>
-  <si>
     <t>Descricao</t>
   </si>
   <si>
@@ -56,21 +50,12 @@
     <t>Valor</t>
   </si>
   <si>
-    <t>Jaguapita</t>
-  </si>
-  <si>
-    <t>Variação do IPCA</t>
-  </si>
-  <si>
     <t>Fonte</t>
   </si>
   <si>
     <t>https://www.bcb.gov.br/controleinflacao/historicometas</t>
   </si>
   <si>
-    <t>Salario Minimo</t>
-  </si>
-  <si>
     <t>https://www.contabeis.com.br/tabelas/salario-minimo/</t>
   </si>
   <si>
@@ -86,9 +71,6 @@
     <t>https://www.bcb.gov.br/content/controleinflacao/controleinflacao_docs/carta_aberta/OF_CIO_823_2022_BCB_SECRE_01.pdf</t>
   </si>
   <si>
-    <t>https://www.planalto.gov.br/ccivil_03/_ato2023-2026/2023/decreto/D11864.htm</t>
-  </si>
-  <si>
     <t>https://www.planalto.gov.br/ccivil_03/_Ato2023-2026/2023/Lei/L14663.htm</t>
   </si>
   <si>
@@ -110,9 +92,6 @@
     <t>https://leis.org/municipais/pr/cafeara/lei/lei-complementar/2025/669/lei-complementar-n-669-2025-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL</t>
   </si>
   <si>
-    <t>https://www.contabeis.com.br/tabelas/salario-minimo/#:~:text=R%24%201.518%2C00-,DECRETO%2012.342/2024,-7%2C51%25</t>
-  </si>
-  <si>
     <t>https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2024/636/lei-ordinaria-n-636-2024-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL</t>
   </si>
   <si>
@@ -146,9 +125,6 @@
     <t>https://www.planalto.gov.br/ccivil_03/_Ato2019-2022/2019/Mpv/mpv916.htm</t>
   </si>
   <si>
-    <t>https://www.planalto.gov.br/ccivil_03/_ato2023-2026/2024/decreto/D12342.htm</t>
-  </si>
-  <si>
     <t>https://www.ibge.gov.br/explica/inflacao.php</t>
   </si>
   <si>
@@ -183,6 +159,42 @@
   </si>
   <si>
     <t>https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2020/2/11/lei-ordinaria-n-11-2020-concede-recomposicao-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-e-ao-prefeito-vice-prefeito-e-secretarios-municipais-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial</t>
+  </si>
+  <si>
+    <t>IPCA</t>
+  </si>
+  <si>
+    <t>Salário Mínimo</t>
+  </si>
+  <si>
+    <t>Primeiro de Maio</t>
+  </si>
+  <si>
+    <t>https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2023/88/876/lei-ordinaria-n-876-2023-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=reajuste+salarial+</t>
+  </si>
+  <si>
+    <t>https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2020/74/739/lei-ordinaria-n-739-2020-dispoe-sobre-a-revisao-geral-anual-do-subsidio-do-prefeito-vice-prefeito-vereadores-secretarios-as-municipais-e-remuneracao-do-s-servidor-es-comissionados-e-estatutario-do-poder-legislativo-do-municipio-de-primeiro-de-maio-e-da-outras-providencias?q=salarial%20</t>
+  </si>
+  <si>
+    <t>https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2025/97/970/lei-ordinaria-n-970-2025-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20</t>
+  </si>
+  <si>
+    <t>https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2024/94/934/lei-ordinaria-n-934-2024-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20</t>
+  </si>
+  <si>
+    <t>https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2022/80/800/lei-ordinaria-n-800-2022-dispoe-sobre-a-revisao-geral-anual-do-subsidio-do-prefeito-vice-prefeito-vereadores-secretarios-as-municipais-e-remuneracao-do-s-servidor-es-comissionados-e-estatutario-do-poder-legislativo-do-municipio-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20</t>
+  </si>
+  <si>
+    <t>https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2021/77/770/lei-ordinaria-n-770-2021-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20</t>
+  </si>
+  <si>
+    <t>Jaguapitã</t>
+  </si>
+  <si>
+    <t>Lupionópolis</t>
+  </si>
+  <si>
+    <t>Centenário do Sul</t>
   </si>
 </sst>
 </file>
@@ -609,42 +621,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A9F774-A2B7-43E0-89BB-A01627A8B05C}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="112.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B2" s="9">
         <v>2025</v>
@@ -653,13 +665,13 @@
         <v>4.2599999999999999E-2</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B3" s="5">
         <v>2024</v>
@@ -668,15 +680,15 @@
         <v>4.8300000000000003E-2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B4" s="5">
         <v>2023</v>
@@ -685,12 +697,12 @@
         <v>4.6199999999999998E-2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B5" s="5">
         <v>2022</v>
@@ -699,15 +711,15 @@
         <v>5.79E-2</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B6" s="5">
         <v>2021</v>
@@ -716,15 +728,15 @@
         <v>0.10059999999999999</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B7" s="5">
         <v>2020</v>
@@ -733,12 +745,12 @@
         <v>4.5199999999999997E-2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B8" s="5">
         <v>2019</v>
@@ -747,7 +759,7 @@
         <v>4.3099999999999999E-2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -756,7 +768,7 @@
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B10" s="5">
         <v>2026</v>
@@ -765,15 +777,13 @@
         <v>6.7900000000000002E-2</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>36</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B11" s="5">
         <v>2025</v>
@@ -782,15 +792,13 @@
         <v>7.51E-2</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>24</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B12" s="5">
         <v>2024</v>
@@ -799,15 +807,13 @@
         <v>6.9699999999999998E-2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B13" s="5">
         <v>2023</v>
@@ -816,15 +822,15 @@
         <v>1.38E-2</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B14" s="5">
         <v>2023</v>
@@ -833,15 +839,15 @@
         <v>7.4300000000000005E-2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B15" s="5">
         <v>2022</v>
@@ -850,15 +856,15 @@
         <v>0.1018</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B16" s="5">
         <v>2021</v>
@@ -867,15 +873,15 @@
         <v>5.2600000000000001E-2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B17" s="5">
         <v>2020</v>
@@ -884,15 +890,15 @@
         <v>5.7999999999999996E-3</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B18" s="5">
         <v>2020</v>
@@ -901,10 +907,10 @@
         <v>4.1099999999999998E-2</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -921,7 +927,7 @@
         <v>6.3700000000000007E-2</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -935,7 +941,7 @@
         <v>4.6199999999999998E-2</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -949,7 +955,7 @@
         <v>5.79E-2</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -963,7 +969,7 @@
         <v>0.10059999999999999</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -977,7 +983,7 @@
         <v>4.5199999999999997E-2</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -991,7 +997,7 @@
         <v>4.48E-2</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -999,7 +1005,7 @@
     </row>
     <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="B27" s="5">
         <v>2025</v>
@@ -1008,12 +1014,12 @@
         <v>0.05</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="B28" s="5">
         <v>2024</v>
@@ -1022,12 +1028,12 @@
         <v>0.05</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="B29" s="5">
         <v>2023</v>
@@ -1036,12 +1042,12 @@
         <v>5.9299999999999999E-2</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="B30" s="5">
         <v>2022</v>
@@ -1050,12 +1056,12 @@
         <v>0.1016</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="B31" s="5">
         <v>2021</v>
@@ -1064,12 +1070,12 @@
         <v>4.5199999999999997E-2</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="B32" s="5">
         <v>2020</v>
@@ -1078,7 +1084,7 @@
         <v>4.48E-2</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1087,7 +1093,7 @@
     </row>
     <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B35" s="5">
         <v>2025</v>
@@ -1096,12 +1102,12 @@
         <v>0.05</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B36" s="5">
         <v>2024</v>
@@ -1110,12 +1116,12 @@
         <v>0.05</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B37" s="5">
         <v>2023</v>
@@ -1124,12 +1130,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B38" s="5">
         <v>2022</v>
@@ -1138,12 +1144,12 @@
         <v>5.45E-2</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B39" s="5">
         <v>2021</v>
@@ -1152,7 +1158,7 @@
     </row>
     <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B40" s="5">
         <v>2020</v>
@@ -1161,7 +1167,7 @@
         <v>4.48E-2</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1169,7 +1175,7 @@
     </row>
     <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B42" s="5">
         <v>2025</v>
@@ -1178,12 +1184,12 @@
         <v>4.1700000000000001E-2</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B43" s="5">
         <v>2024</v>
@@ -1192,12 +1198,12 @@
         <v>3.8199999999999998E-2</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B44" s="5">
         <v>2023</v>
@@ -1206,12 +1212,12 @@
         <v>5.7099999999999998E-2</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B45" s="5">
         <v>2022</v>
@@ -1220,12 +1226,12 @@
         <v>0.106</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B46" s="5">
         <v>2021</v>
@@ -1234,12 +1240,12 @@
         <v>5.5300000000000002E-2</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B47" s="5">
         <v>2020</v>
@@ -1248,14 +1254,95 @@
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C48" s="7"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C49" s="7"/>
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="5">
+        <v>2025</v>
+      </c>
+      <c r="C49" s="7">
+        <v>4.8300000000000003E-2</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="5">
+        <v>2024</v>
+      </c>
+      <c r="C50" s="7">
+        <v>0.11460000000000001</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" s="5">
+        <v>2023</v>
+      </c>
+      <c r="C51" s="7">
+        <v>0.1263</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52" s="5">
+        <v>2022</v>
+      </c>
+      <c r="C52" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="5">
+        <v>2021</v>
+      </c>
+      <c r="C53" s="7">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" s="5">
+        <v>2020</v>
+      </c>
+      <c r="C54" s="7">
+        <v>7.3178999999999994E-2</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1269,35 +1356,38 @@
     <hyperlink ref="E14" r:id="rId8" xr:uid="{CE999FD0-8CBC-4BEA-84BE-95B4E1C3A1C5}"/>
     <hyperlink ref="D22" r:id="rId9" display="https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2023/609/lei-ordinaria-n-609-2023-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias" xr:uid="{C3275B82-C56D-4C85-BA27-2F2BD690BB16}"/>
     <hyperlink ref="D20" r:id="rId10" display="https://leis.org/municipais/pr/cafeara/lei/lei-complementar/2025/669/lei-complementar-n-669-2025-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL" xr:uid="{A7EAD4F8-68E0-41D4-AE50-5A0B782E8B8F}"/>
-    <hyperlink ref="E12" r:id="rId11" xr:uid="{4DFD4716-342F-45B9-9C77-D8607A1A0FD9}"/>
-    <hyperlink ref="E11" r:id="rId12" location=":~:text=R%24%201.518%2C00-,DECRETO%2012.342/2024,-7%2C51%25" xr:uid="{3CC176B3-F827-4927-A37E-47345EAB6DDB}"/>
-    <hyperlink ref="D21" r:id="rId13" display="https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2024/636/lei-ordinaria-n-636-2024-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL" xr:uid="{23D66F80-65EE-4A0F-8144-F36DB20450EF}"/>
-    <hyperlink ref="D23" r:id="rId14" display="https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2022/587/lei-ordinaria-n-587-2022-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL" xr:uid="{1B38F967-CA98-456B-9E39-53D8B29C2593}"/>
-    <hyperlink ref="D24" r:id="rId15" display="https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2021/563/lei-ordinaria-n-563-2021-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL" xr:uid="{2F2E9EFC-04E5-4D6C-ADAE-3D1C1FE4D8C2}"/>
-    <hyperlink ref="D25" r:id="rId16" display="https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2020/542/lei-ordinaria-n-542-2020-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-revisao-salarial-aos-servidores-publicos-municipais-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL" xr:uid="{CE150FB9-81B7-4D95-A8CF-6EF4FEC69817}"/>
-    <hyperlink ref="D27" r:id="rId17" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2025/325/3248/lei-ordinaria-n-3248-2025-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-com-excecao-dos-subsidios-dos-agentes-politicos?q=reajuste" xr:uid="{14532045-718C-41E1-8B54-50EFD37FBDB7}"/>
-    <hyperlink ref="D28" r:id="rId18" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2024/322/3211/lei-ordinaria-n-3211-2024-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-inclusive-sobre-os-subsidios-dos-agentes-politicos?q=reajuste" xr:uid="{38AE6B04-78B2-4EB9-9571-DB2D521C73B5}"/>
-    <hyperlink ref="D29" r:id="rId19" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2023/317/3170/lei-ordinaria-n-3170-2023-autoriza-a-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-inclusive-sobre-os-subsidios-dos-agentes-politicos?q=reajuste" xr:uid="{4CF69429-E3A8-42D6-85E9-C1B4DF636DEA}"/>
-    <hyperlink ref="D30" r:id="rId20" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2022/314/3132/lei-ordinaria-n-3132-2022-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-inclusive-sobre-os-subsidios-dos-agentes-politicos?q=reajuste" xr:uid="{55BFE9D4-B84C-4424-B8D7-86FC64A9AB3E}"/>
-    <hyperlink ref="D31" r:id="rId21" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2021/310/3097/lei-ordinaria-n-3097-2021-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao?q=reajuste" xr:uid="{87876156-98C2-4000-91CE-7C8AD0B3476E}"/>
-    <hyperlink ref="D32" r:id="rId22" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2020/305/3045/lei-ordinaria-n-3045-2020-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-inclusive-sobre-os-subsidios-dos-agentes-politicos-bem-como-adequa-o-salario-dos-servidores-do-quadro-do-magisterio-publico-municipal-ao-piso-salarial-profissional-nacional?q=reajuste" xr:uid="{DF65B76A-65AA-4C35-A537-F477C0AB6BF4}"/>
-    <hyperlink ref="E18" r:id="rId23" xr:uid="{EC4616F6-7680-425A-9B5B-FA1377623831}"/>
-    <hyperlink ref="D10" r:id="rId24" xr:uid="{5B0B0D6A-84BF-4334-B8E3-04EFE33A5016}"/>
-    <hyperlink ref="E10" r:id="rId25" xr:uid="{02C5A970-ED41-49F9-A0EF-CA25BAD69096}"/>
-    <hyperlink ref="D2" r:id="rId26" xr:uid="{5300EFF3-C77D-4044-9FEE-10FEE221CCA5}"/>
-    <hyperlink ref="D35" r:id="rId27" xr:uid="{0198FF07-6ABC-4FE0-BC94-9626A092EF1E}"/>
-    <hyperlink ref="D36" r:id="rId28" xr:uid="{9B9DADFC-147D-439F-A89B-8D7EC2EFFA45}"/>
-    <hyperlink ref="D37" r:id="rId29" xr:uid="{7B4312A5-B4D6-48C3-9967-D4A547A0F189}"/>
-    <hyperlink ref="D38" r:id="rId30" xr:uid="{11C55EFF-5E2A-48DD-A430-CB5E5C32EF37}"/>
-    <hyperlink ref="D40" r:id="rId31" xr:uid="{B555F1DF-7AE0-4CE3-A746-A72DB71A3814}"/>
-    <hyperlink ref="D42" r:id="rId32" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2025/1/3/lei-ordinaria-n-3-2025-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{79AF655C-919A-4B59-8D63-6E9B71A0DFD8}"/>
-    <hyperlink ref="D43" r:id="rId33" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2024/1/6/lei-ordinaria-n-6-2024-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-e-recomposicao-inflacionaria-aos-agentes-politicos-do-poder-executivo-prefeito-vice-prefeito-e-secretarios-municipais-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{28DF2AEC-02FD-4904-92E4-8F1A46B7C53A}"/>
-    <hyperlink ref="D44" r:id="rId34" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2023/1/3/lei-ordinaria-n-3-2023-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-e-recomposicao-inflacionaria-aos-agentes-politicos-do-poder-executivo-prefeito-vice-prefeito-e-secretarios-municipais-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{D52BDBF7-13A5-4A80-A127-116B587657FB}"/>
-    <hyperlink ref="D45" r:id="rId35" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2022/1/5/lei-ordinaria-n-5-2022-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{3E75ABFE-1194-4B2F-AF68-D20DEC412ED8}"/>
-    <hyperlink ref="D46" r:id="rId36" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2021/1/5/lei-ordinaria-n-5-2021-concede-recomposicao-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{4FC8FEEE-0401-4369-8921-ED4B51F5562D}"/>
-    <hyperlink ref="D47" r:id="rId37" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2020/2/11/lei-ordinaria-n-11-2020-concede-recomposicao-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-e-ao-prefeito-vice-prefeito-e-secretarios-municipais-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{4D8E764E-22B9-4B1F-A195-598C7E088B03}"/>
+    <hyperlink ref="D21" r:id="rId11" display="https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2024/636/lei-ordinaria-n-636-2024-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL" xr:uid="{23D66F80-65EE-4A0F-8144-F36DB20450EF}"/>
+    <hyperlink ref="D23" r:id="rId12" display="https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2022/587/lei-ordinaria-n-587-2022-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL" xr:uid="{1B38F967-CA98-456B-9E39-53D8B29C2593}"/>
+    <hyperlink ref="D24" r:id="rId13" display="https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2021/563/lei-ordinaria-n-563-2021-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL" xr:uid="{2F2E9EFC-04E5-4D6C-ADAE-3D1C1FE4D8C2}"/>
+    <hyperlink ref="D25" r:id="rId14" display="https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2020/542/lei-ordinaria-n-542-2020-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-revisao-salarial-aos-servidores-publicos-municipais-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL" xr:uid="{CE150FB9-81B7-4D95-A8CF-6EF4FEC69817}"/>
+    <hyperlink ref="D27" r:id="rId15" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2025/325/3248/lei-ordinaria-n-3248-2025-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-com-excecao-dos-subsidios-dos-agentes-politicos?q=reajuste" xr:uid="{14532045-718C-41E1-8B54-50EFD37FBDB7}"/>
+    <hyperlink ref="D28" r:id="rId16" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2024/322/3211/lei-ordinaria-n-3211-2024-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-inclusive-sobre-os-subsidios-dos-agentes-politicos?q=reajuste" xr:uid="{38AE6B04-78B2-4EB9-9571-DB2D521C73B5}"/>
+    <hyperlink ref="D29" r:id="rId17" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2023/317/3170/lei-ordinaria-n-3170-2023-autoriza-a-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-inclusive-sobre-os-subsidios-dos-agentes-politicos?q=reajuste" xr:uid="{4CF69429-E3A8-42D6-85E9-C1B4DF636DEA}"/>
+    <hyperlink ref="D30" r:id="rId18" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2022/314/3132/lei-ordinaria-n-3132-2022-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-inclusive-sobre-os-subsidios-dos-agentes-politicos?q=reajuste" xr:uid="{55BFE9D4-B84C-4424-B8D7-86FC64A9AB3E}"/>
+    <hyperlink ref="D31" r:id="rId19" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2021/310/3097/lei-ordinaria-n-3097-2021-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao?q=reajuste" xr:uid="{87876156-98C2-4000-91CE-7C8AD0B3476E}"/>
+    <hyperlink ref="D32" r:id="rId20" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2020/305/3045/lei-ordinaria-n-3045-2020-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-inclusive-sobre-os-subsidios-dos-agentes-politicos-bem-como-adequa-o-salario-dos-servidores-do-quadro-do-magisterio-publico-municipal-ao-piso-salarial-profissional-nacional?q=reajuste" xr:uid="{DF65B76A-65AA-4C35-A537-F477C0AB6BF4}"/>
+    <hyperlink ref="E18" r:id="rId21" xr:uid="{EC4616F6-7680-425A-9B5B-FA1377623831}"/>
+    <hyperlink ref="D10" r:id="rId22" xr:uid="{5B0B0D6A-84BF-4334-B8E3-04EFE33A5016}"/>
+    <hyperlink ref="D2" r:id="rId23" xr:uid="{5300EFF3-C77D-4044-9FEE-10FEE221CCA5}"/>
+    <hyperlink ref="D35" r:id="rId24" xr:uid="{0198FF07-6ABC-4FE0-BC94-9626A092EF1E}"/>
+    <hyperlink ref="D36" r:id="rId25" xr:uid="{9B9DADFC-147D-439F-A89B-8D7EC2EFFA45}"/>
+    <hyperlink ref="D37" r:id="rId26" xr:uid="{7B4312A5-B4D6-48C3-9967-D4A547A0F189}"/>
+    <hyperlink ref="D38" r:id="rId27" xr:uid="{11C55EFF-5E2A-48DD-A430-CB5E5C32EF37}"/>
+    <hyperlink ref="D40" r:id="rId28" xr:uid="{B555F1DF-7AE0-4CE3-A746-A72DB71A3814}"/>
+    <hyperlink ref="D42" r:id="rId29" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2025/1/3/lei-ordinaria-n-3-2025-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{79AF655C-919A-4B59-8D63-6E9B71A0DFD8}"/>
+    <hyperlink ref="D43" r:id="rId30" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2024/1/6/lei-ordinaria-n-6-2024-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-e-recomposicao-inflacionaria-aos-agentes-politicos-do-poder-executivo-prefeito-vice-prefeito-e-secretarios-municipais-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{28DF2AEC-02FD-4904-92E4-8F1A46B7C53A}"/>
+    <hyperlink ref="D44" r:id="rId31" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2023/1/3/lei-ordinaria-n-3-2023-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-e-recomposicao-inflacionaria-aos-agentes-politicos-do-poder-executivo-prefeito-vice-prefeito-e-secretarios-municipais-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{D52BDBF7-13A5-4A80-A127-116B587657FB}"/>
+    <hyperlink ref="D45" r:id="rId32" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2022/1/5/lei-ordinaria-n-5-2022-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{3E75ABFE-1194-4B2F-AF68-D20DEC412ED8}"/>
+    <hyperlink ref="D46" r:id="rId33" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2021/1/5/lei-ordinaria-n-5-2021-concede-recomposicao-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{4FC8FEEE-0401-4369-8921-ED4B51F5562D}"/>
+    <hyperlink ref="D47" r:id="rId34" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2020/2/11/lei-ordinaria-n-11-2020-concede-recomposicao-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-e-ao-prefeito-vice-prefeito-e-secretarios-municipais-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{4D8E764E-22B9-4B1F-A195-598C7E088B03}"/>
+    <hyperlink ref="D51" r:id="rId35" xr:uid="{469628B4-8B6D-46C9-A62E-832B5D06C62E}"/>
+    <hyperlink ref="D54" r:id="rId36" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2020/74/739/lei-ordinaria-n-739-2020-dispoe-sobre-a-revisao-geral-anual-do-subsidio-do-prefeito-vice-prefeito-vereadores-secretarios-as-municipais-e-remuneracao-do-s-servidor-es-comissionados-e-estatutario-do-poder-legislativo-do-municipio-de-primeiro-de-maio-e-da-outras-providencias?q=salarial%20" xr:uid="{8F367E47-ABB7-4AAB-A611-4BB40BDA61A3}"/>
+    <hyperlink ref="D49" r:id="rId37" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2025/97/970/lei-ordinaria-n-970-2025-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{9C1E9D0B-D3E4-4ECB-928C-3AB9384788C0}"/>
+    <hyperlink ref="D50" r:id="rId38" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2024/94/934/lei-ordinaria-n-934-2024-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{AF964D4D-7701-48C8-898F-A6225D73AC79}"/>
+    <hyperlink ref="D52" r:id="rId39" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2022/80/800/lei-ordinaria-n-800-2022-dispoe-sobre-a-revisao-geral-anual-do-subsidio-do-prefeito-vice-prefeito-vereadores-secretarios-as-municipais-e-remuneracao-do-s-servidor-es-comissionados-e-estatutario-do-poder-legislativo-do-municipio-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{98F545B3-8D3D-44B1-AB35-4AC2759963EB}"/>
+    <hyperlink ref="D53" r:id="rId40" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2021/77/770/lei-ordinaria-n-770-2021-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{C52DDB23-FB88-489B-BD74-E79A0801ADF5}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId38"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId41"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added grafico de composição
</commit_message>
<xml_diff>
--- a/data/dados.xlsx
+++ b/data/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\reajuste\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD06113-323D-46EF-B382-A2E642F3035C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8F8F6B-5A0E-421E-847B-65320EDAEDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{BE2A1F3B-6535-41F1-9783-CEB15E5262F6}"/>
   </bookViews>
@@ -223,12 +223,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF606060"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -238,14 +232,22 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="10"/>
-      <color theme="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF333333"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -269,9 +271,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -284,18 +286,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -633,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A9F774-A2B7-43E0-89BB-A01627A8B05C}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -668,13 +667,13 @@
       <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="6">
         <v>2025</v>
       </c>
       <c r="C2" s="7">
         <v>4.2599999999999999E-2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="1"/>
@@ -692,7 +691,7 @@
       <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -723,7 +722,7 @@
       <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -740,7 +739,7 @@
       <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -786,10 +785,10 @@
       <c r="C10" s="7">
         <v>6.7900000000000002E-2</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
@@ -804,7 +803,7 @@
       <c r="D11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="8"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
@@ -819,7 +818,7 @@
       <c r="D12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
@@ -834,7 +833,7 @@
       <c r="D13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -851,7 +850,7 @@
       <c r="D14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -868,7 +867,7 @@
       <c r="D15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -885,7 +884,7 @@
       <c r="D16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -902,7 +901,7 @@
       <c r="D17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -919,7 +918,7 @@
       <c r="D18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="8" t="s">
         <v>28</v>
       </c>
     </row>
@@ -936,7 +935,7 @@
       <c r="C20" s="7">
         <v>0.1</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -950,7 +949,7 @@
       <c r="C21" s="7">
         <v>0.05</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="9" t="s">
         <v>18</v>
       </c>
     </row>
@@ -964,7 +963,7 @@
       <c r="C22" s="7">
         <v>0.2</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -978,7 +977,7 @@
       <c r="C23" s="7">
         <v>0.16059999999999999</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -992,7 +991,7 @@
       <c r="C24" s="7">
         <v>4.5199999999999997E-2</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="9" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1006,7 +1005,7 @@
       <c r="C25" s="7">
         <v>0.05</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1023,7 +1022,7 @@
       <c r="C27" s="7">
         <v>0.05</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1037,7 +1036,7 @@
       <c r="C28" s="7">
         <v>0.05</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1051,7 +1050,7 @@
       <c r="C29" s="7">
         <v>5.9299999999999999E-2</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="8" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1065,7 +1064,7 @@
       <c r="C30" s="7">
         <v>0.1016</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="8" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1079,7 +1078,7 @@
       <c r="C31" s="7">
         <v>4.5199999999999997E-2</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1093,13 +1092,13 @@
       <c r="C32" s="7">
         <v>4.48E-2</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="C33" s="7"/>
-      <c r="D33" s="6"/>
+      <c r="D33" s="8"/>
     </row>
     <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
@@ -1111,7 +1110,7 @@
       <c r="C34" s="7">
         <v>0.05</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="8" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1125,7 +1124,7 @@
       <c r="C35" s="7">
         <v>0.05</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="8" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1139,7 +1138,7 @@
       <c r="C36" s="7">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="8" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1153,7 +1152,7 @@
       <c r="C37" s="7">
         <v>5.45E-2</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="8" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1176,7 +1175,7 @@
       <c r="C39" s="7">
         <v>4.48E-2</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1193,7 +1192,7 @@
       <c r="C41" s="7">
         <v>0.05</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="8" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1207,7 +1206,7 @@
       <c r="C42" s="7">
         <v>0.05</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="8" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1221,7 +1220,7 @@
       <c r="C43" s="7">
         <v>0.14949999999999999</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="8" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1235,7 +1234,7 @@
       <c r="C44" s="7">
         <v>0.15</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="8" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1249,7 +1248,7 @@
       <c r="C45" s="7">
         <v>5.5300000000000002E-2</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" s="8" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1263,7 +1262,7 @@
       <c r="C46" s="7">
         <v>2.2499999999999999E-2</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D46" s="8" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1280,7 +1279,7 @@
       <c r="C48" s="7">
         <v>4.8300000000000003E-2</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D48" s="8" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1294,7 +1293,7 @@
       <c r="C49" s="7">
         <v>0.11460000000000001</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D49" s="8" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1308,7 +1307,7 @@
       <c r="C50" s="7">
         <v>0.1263</v>
       </c>
-      <c r="D50" s="6" t="s">
+      <c r="D50" s="8" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1322,7 +1321,7 @@
       <c r="C51" s="7">
         <v>0.15</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="D51" s="8" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1336,7 +1335,7 @@
       <c r="C52" s="7">
         <v>4.5199999999999997E-2</v>
       </c>
-      <c r="D52" s="6" t="s">
+      <c r="D52" s="8" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1350,14 +1349,14 @@
       <c r="C53" s="7">
         <v>7.3178999999999994E-2</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D53" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
       <c r="B57" s="10"/>
-      <c r="C57" s="11"/>
+      <c r="C57" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
added segunda lei de lupionopolis
</commit_message>
<xml_diff>
--- a/data/dados.xlsx
+++ b/data/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\reajuste\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8F8F6B-5A0E-421E-847B-65320EDAEDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCAA2FA-032F-404B-880D-C7E7823F95AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{BE2A1F3B-6535-41F1-9783-CEB15E5262F6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="54">
   <si>
     <t>Cafeara</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>Centenário do Sul</t>
+  </si>
+  <si>
+    <t>https://leggicomunali.it/a/pr/l/lupionopolis/lei-ordinaria/2022/1/1/lei-ordinaria-n-1-2022-dispoe-sobre-a-reposicao-salarial-dos-servidores-publicos-municipais-de-lupionopolis?q=reposi%E7%E3o%20salarial</t>
   </si>
 </sst>
 </file>
@@ -273,7 +276,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -295,6 +298,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -630,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A9F774-A2B7-43E0-89BB-A01627A8B05C}">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D29" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1152,62 +1156,62 @@
       <c r="C37" s="7">
         <v>5.45E-2</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B38" s="5">
-        <v>2021</v>
-      </c>
-      <c r="C38" s="7"/>
-    </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>2022</v>
+      </c>
+      <c r="C38" s="7">
+        <v>0.1016</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B39" s="5">
+        <v>2021</v>
+      </c>
+      <c r="C39" s="7"/>
+    </row>
+    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="5">
         <v>2020</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C40" s="7">
         <v>4.48E-2</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D40" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C40" s="7"/>
-    </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" s="5">
-        <v>2025</v>
-      </c>
-      <c r="C41" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>35</v>
-      </c>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C41" s="7"/>
     </row>
     <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B42" s="5">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="C42" s="7">
         <v>0.05</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1215,13 +1219,13 @@
         <v>50</v>
       </c>
       <c r="B43" s="5">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C43" s="7">
-        <v>0.14949999999999999</v>
+        <v>0.05</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1229,13 +1233,13 @@
         <v>50</v>
       </c>
       <c r="B44" s="5">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C44" s="7">
-        <v>0.15</v>
+        <v>0.14949999999999999</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1243,13 +1247,13 @@
         <v>50</v>
       </c>
       <c r="B45" s="5">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C45" s="7">
-        <v>5.5300000000000002E-2</v>
+        <v>0.15</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1257,44 +1261,44 @@
         <v>50</v>
       </c>
       <c r="B46" s="5">
+        <v>2021</v>
+      </c>
+      <c r="C46" s="7">
+        <v>5.5300000000000002E-2</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="5">
         <v>2020</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C47" s="7">
         <v>2.2499999999999999E-2</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D47" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C47" s="7"/>
-    </row>
-    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B48" s="5">
-        <v>2025</v>
-      </c>
-      <c r="C48" s="7">
-        <v>4.8300000000000003E-2</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>46</v>
-      </c>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C48" s="7"/>
     </row>
     <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B49" s="5">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="C49" s="7">
-        <v>0.11460000000000001</v>
+        <v>4.8300000000000003E-2</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1302,13 +1306,13 @@
         <v>43</v>
       </c>
       <c r="B50" s="5">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C50" s="7">
-        <v>0.1263</v>
+        <v>0.11460000000000001</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1316,13 +1320,13 @@
         <v>43</v>
       </c>
       <c r="B51" s="5">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C51" s="7">
-        <v>0.15</v>
+        <v>0.1263</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1330,13 +1334,13 @@
         <v>43</v>
       </c>
       <c r="B52" s="5">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C52" s="7">
-        <v>4.5199999999999997E-2</v>
+        <v>0.15</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1344,19 +1348,33 @@
         <v>43</v>
       </c>
       <c r="B53" s="5">
+        <v>2021</v>
+      </c>
+      <c r="C53" s="7">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" s="5">
         <v>2020</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C54" s="7">
         <v>7.3178999999999994E-2</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D54" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="10"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="7"/>
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1386,22 +1404,23 @@
     <hyperlink ref="D34" r:id="rId24" xr:uid="{0198FF07-6ABC-4FE0-BC94-9626A092EF1E}"/>
     <hyperlink ref="D35" r:id="rId25" xr:uid="{9B9DADFC-147D-439F-A89B-8D7EC2EFFA45}"/>
     <hyperlink ref="D36" r:id="rId26" xr:uid="{7B4312A5-B4D6-48C3-9967-D4A547A0F189}"/>
-    <hyperlink ref="D37" r:id="rId27" xr:uid="{11C55EFF-5E2A-48DD-A430-CB5E5C32EF37}"/>
-    <hyperlink ref="D39" r:id="rId28" xr:uid="{B555F1DF-7AE0-4CE3-A746-A72DB71A3814}"/>
-    <hyperlink ref="D41" r:id="rId29" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2025/1/3/lei-ordinaria-n-3-2025-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{79AF655C-919A-4B59-8D63-6E9B71A0DFD8}"/>
-    <hyperlink ref="D42" r:id="rId30" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2024/1/6/lei-ordinaria-n-6-2024-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-e-recomposicao-inflacionaria-aos-agentes-politicos-do-poder-executivo-prefeito-vice-prefeito-e-secretarios-municipais-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{28DF2AEC-02FD-4904-92E4-8F1A46B7C53A}"/>
-    <hyperlink ref="D43" r:id="rId31" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2023/1/3/lei-ordinaria-n-3-2023-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-e-recomposicao-inflacionaria-aos-agentes-politicos-do-poder-executivo-prefeito-vice-prefeito-e-secretarios-municipais-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{D52BDBF7-13A5-4A80-A127-116B587657FB}"/>
-    <hyperlink ref="D44" r:id="rId32" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2022/1/5/lei-ordinaria-n-5-2022-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{3E75ABFE-1194-4B2F-AF68-D20DEC412ED8}"/>
-    <hyperlink ref="D45" r:id="rId33" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2021/1/5/lei-ordinaria-n-5-2021-concede-recomposicao-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{4FC8FEEE-0401-4369-8921-ED4B51F5562D}"/>
-    <hyperlink ref="D46" r:id="rId34" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2020/2/11/lei-ordinaria-n-11-2020-concede-recomposicao-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-e-ao-prefeito-vice-prefeito-e-secretarios-municipais-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{4D8E764E-22B9-4B1F-A195-598C7E088B03}"/>
-    <hyperlink ref="D50" r:id="rId35" xr:uid="{469628B4-8B6D-46C9-A62E-832B5D06C62E}"/>
-    <hyperlink ref="D53" r:id="rId36" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2020/74/739/lei-ordinaria-n-739-2020-dispoe-sobre-a-revisao-geral-anual-do-subsidio-do-prefeito-vice-prefeito-vereadores-secretarios-as-municipais-e-remuneracao-do-s-servidor-es-comissionados-e-estatutario-do-poder-legislativo-do-municipio-de-primeiro-de-maio-e-da-outras-providencias?q=salarial%20" xr:uid="{8F367E47-ABB7-4AAB-A611-4BB40BDA61A3}"/>
-    <hyperlink ref="D48" r:id="rId37" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2025/97/970/lei-ordinaria-n-970-2025-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{9C1E9D0B-D3E4-4ECB-928C-3AB9384788C0}"/>
-    <hyperlink ref="D49" r:id="rId38" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2024/94/934/lei-ordinaria-n-934-2024-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{AF964D4D-7701-48C8-898F-A6225D73AC79}"/>
-    <hyperlink ref="D51" r:id="rId39" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2022/80/800/lei-ordinaria-n-800-2022-dispoe-sobre-a-revisao-geral-anual-do-subsidio-do-prefeito-vice-prefeito-vereadores-secretarios-as-municipais-e-remuneracao-do-s-servidor-es-comissionados-e-estatutario-do-poder-legislativo-do-municipio-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{98F545B3-8D3D-44B1-AB35-4AC2759963EB}"/>
-    <hyperlink ref="D52" r:id="rId40" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2021/77/770/lei-ordinaria-n-770-2021-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{C52DDB23-FB88-489B-BD74-E79A0801ADF5}"/>
+    <hyperlink ref="D40" r:id="rId27" xr:uid="{B555F1DF-7AE0-4CE3-A746-A72DB71A3814}"/>
+    <hyperlink ref="D42" r:id="rId28" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2025/1/3/lei-ordinaria-n-3-2025-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{79AF655C-919A-4B59-8D63-6E9B71A0DFD8}"/>
+    <hyperlink ref="D43" r:id="rId29" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2024/1/6/lei-ordinaria-n-6-2024-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-e-recomposicao-inflacionaria-aos-agentes-politicos-do-poder-executivo-prefeito-vice-prefeito-e-secretarios-municipais-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{28DF2AEC-02FD-4904-92E4-8F1A46B7C53A}"/>
+    <hyperlink ref="D44" r:id="rId30" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2023/1/3/lei-ordinaria-n-3-2023-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-e-recomposicao-inflacionaria-aos-agentes-politicos-do-poder-executivo-prefeito-vice-prefeito-e-secretarios-municipais-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{D52BDBF7-13A5-4A80-A127-116B587657FB}"/>
+    <hyperlink ref="D45" r:id="rId31" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2022/1/5/lei-ordinaria-n-5-2022-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{3E75ABFE-1194-4B2F-AF68-D20DEC412ED8}"/>
+    <hyperlink ref="D46" r:id="rId32" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2021/1/5/lei-ordinaria-n-5-2021-concede-recomposicao-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{4FC8FEEE-0401-4369-8921-ED4B51F5562D}"/>
+    <hyperlink ref="D47" r:id="rId33" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2020/2/11/lei-ordinaria-n-11-2020-concede-recomposicao-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-e-ao-prefeito-vice-prefeito-e-secretarios-municipais-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{4D8E764E-22B9-4B1F-A195-598C7E088B03}"/>
+    <hyperlink ref="D51" r:id="rId34" xr:uid="{469628B4-8B6D-46C9-A62E-832B5D06C62E}"/>
+    <hyperlink ref="D54" r:id="rId35" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2020/74/739/lei-ordinaria-n-739-2020-dispoe-sobre-a-revisao-geral-anual-do-subsidio-do-prefeito-vice-prefeito-vereadores-secretarios-as-municipais-e-remuneracao-do-s-servidor-es-comissionados-e-estatutario-do-poder-legislativo-do-municipio-de-primeiro-de-maio-e-da-outras-providencias?q=salarial%20" xr:uid="{8F367E47-ABB7-4AAB-A611-4BB40BDA61A3}"/>
+    <hyperlink ref="D49" r:id="rId36" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2025/97/970/lei-ordinaria-n-970-2025-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{9C1E9D0B-D3E4-4ECB-928C-3AB9384788C0}"/>
+    <hyperlink ref="D50" r:id="rId37" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2024/94/934/lei-ordinaria-n-934-2024-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{AF964D4D-7701-48C8-898F-A6225D73AC79}"/>
+    <hyperlink ref="D52" r:id="rId38" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2022/80/800/lei-ordinaria-n-800-2022-dispoe-sobre-a-revisao-geral-anual-do-subsidio-do-prefeito-vice-prefeito-vereadores-secretarios-as-municipais-e-remuneracao-do-s-servidor-es-comissionados-e-estatutario-do-poder-legislativo-do-municipio-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{98F545B3-8D3D-44B1-AB35-4AC2759963EB}"/>
+    <hyperlink ref="D53" r:id="rId39" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2021/77/770/lei-ordinaria-n-770-2021-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{C52DDB23-FB88-489B-BD74-E79A0801ADF5}"/>
+    <hyperlink ref="D38" r:id="rId40" xr:uid="{878A7E66-55B4-4DAF-8A75-A1CF624BBEC7}"/>
+    <hyperlink ref="D37" r:id="rId41" xr:uid="{47F34AB3-0A0A-412F-8FE1-03EF5CACC9CA}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId41"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId42"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added mapa e agrupamentos de dados
</commit_message>
<xml_diff>
--- a/data/dados.xlsx
+++ b/data/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\reajuste\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED381CD-B075-4D03-983A-7F8D2E73DCB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1424D274-2029-4EF0-9A99-C154FED1D0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{BE2A1F3B-6535-41F1-9783-CEB15E5262F6}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="1" xr2:uid="{BE2A1F3B-6535-41F1-9783-CEB15E5262F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="65">
   <si>
     <t>Cafeara</t>
   </si>
@@ -228,14 +228,17 @@
     <t>Porecatu</t>
   </si>
   <si>
-    <t>Florestopolis</t>
+    <t>cod_ibge</t>
+  </si>
+  <si>
+    <t>Florestópolis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +282,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0054A3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -301,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -323,6 +332,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -658,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A9F774-A2B7-43E0-89BB-A01627A8B05C}">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:XFD62"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D23:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -669,12 +688,13 @@
     <col min="1" max="1" width="20.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" style="5" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="112.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="3"/>
+    <col min="4" max="4" width="16" style="13" customWidth="1"/>
+    <col min="5" max="5" width="255.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="112.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -684,14 +704,17 @@
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
@@ -701,12 +724,13 @@
       <c r="C2" s="7">
         <v>4.2599999999999999E-2</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>41</v>
       </c>
@@ -716,14 +740,14 @@
       <c r="C3" s="7">
         <v>4.8300000000000003E-2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>41</v>
       </c>
@@ -733,11 +757,11 @@
       <c r="C4" s="7">
         <v>4.6199999999999998E-2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>41</v>
       </c>
@@ -747,14 +771,14 @@
       <c r="C5" s="7">
         <v>5.79E-2</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>41</v>
       </c>
@@ -764,14 +788,14 @@
       <c r="C6" s="7">
         <v>0.10059999999999999</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
@@ -781,11 +805,11 @@
       <c r="C7" s="7">
         <v>4.5199999999999997E-2</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>41</v>
       </c>
@@ -795,15 +819,15 @@
       <c r="C8" s="7">
         <v>4.3099999999999999E-2</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
@@ -813,12 +837,12 @@
       <c r="C10" s="7">
         <v>6.7900000000000002E-2</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>42</v>
       </c>
@@ -828,12 +852,12 @@
       <c r="C11" s="7">
         <v>7.51E-2</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>42</v>
       </c>
@@ -843,12 +867,12 @@
       <c r="C12" s="7">
         <v>6.9699999999999998E-2</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>42</v>
       </c>
@@ -858,14 +882,14 @@
       <c r="C13" s="7">
         <v>1.38E-2</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="F13" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>42</v>
       </c>
@@ -875,14 +899,14 @@
       <c r="C14" s="7">
         <v>7.4300000000000005E-2</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="F14" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
@@ -892,14 +916,14 @@
       <c r="C15" s="7">
         <v>0.1018</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="F15" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>42</v>
       </c>
@@ -909,14 +933,14 @@
       <c r="C16" s="7">
         <v>5.2600000000000001E-2</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="F16" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>42</v>
       </c>
@@ -926,14 +950,14 @@
       <c r="C17" s="7">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="F17" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>42</v>
       </c>
@@ -943,17 +967,17 @@
       <c r="C18" s="7">
         <v>4.1099999999999998E-2</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="F18" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>0</v>
       </c>
@@ -963,11 +987,14 @@
       <c r="C20" s="7">
         <v>0.1</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="14">
+        <v>4103404</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>0</v>
       </c>
@@ -977,11 +1004,14 @@
       <c r="C21" s="7">
         <v>0.05</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="14">
+        <v>4103404</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>0</v>
       </c>
@@ -991,11 +1021,14 @@
       <c r="C22" s="7">
         <v>0.2</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="14">
+        <v>4103404</v>
+      </c>
+      <c r="E22" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>0</v>
       </c>
@@ -1005,11 +1038,14 @@
       <c r="C23" s="7">
         <v>0.16059999999999999</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="14">
+        <v>4103404</v>
+      </c>
+      <c r="E23" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>0</v>
       </c>
@@ -1019,11 +1055,14 @@
       <c r="C24" s="7">
         <v>4.5199999999999997E-2</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="14">
+        <v>4103404</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>0</v>
       </c>
@@ -1033,14 +1072,18 @@
       <c r="C25" s="7">
         <v>0.05</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="14">
+        <v>4103404</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C26" s="7"/>
-    </row>
-    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="D26" s="14"/>
+    </row>
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>52</v>
       </c>
@@ -1050,11 +1093,14 @@
       <c r="C27" s="7">
         <v>0.05</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="14">
+        <v>4105102</v>
+      </c>
+      <c r="E27" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>52</v>
       </c>
@@ -1064,11 +1110,14 @@
       <c r="C28" s="7">
         <v>0.05</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="14">
+        <v>4105102</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>52</v>
       </c>
@@ -1078,11 +1127,14 @@
       <c r="C29" s="7">
         <v>5.9299999999999999E-2</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="14">
+        <v>4105102</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>52</v>
       </c>
@@ -1092,11 +1144,14 @@
       <c r="C30" s="7">
         <v>0.1016</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="14">
+        <v>4105102</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>52</v>
       </c>
@@ -1106,11 +1161,14 @@
       <c r="C31" s="7">
         <v>4.5199999999999997E-2</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="14">
+        <v>4105102</v>
+      </c>
+      <c r="E31" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>52</v>
       </c>
@@ -1120,15 +1178,19 @@
       <c r="C32" s="7">
         <v>4.48E-2</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="14">
+        <v>4105102</v>
+      </c>
+      <c r="E32" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="C33" s="7"/>
-      <c r="D33" s="8"/>
-    </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D33" s="14"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>51</v>
       </c>
@@ -1138,11 +1200,14 @@
       <c r="C34" s="7">
         <v>0.05</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="14">
+        <v>4113809</v>
+      </c>
+      <c r="E34" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>51</v>
       </c>
@@ -1152,11 +1217,14 @@
       <c r="C35" s="7">
         <v>0.05</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="14">
+        <v>4113809</v>
+      </c>
+      <c r="E35" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>51</v>
       </c>
@@ -1166,11 +1234,14 @@
       <c r="C36" s="7">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="14">
+        <v>4113809</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>51</v>
       </c>
@@ -1180,11 +1251,14 @@
       <c r="C37" s="7">
         <v>5.45E-2</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="14">
+        <v>4113809</v>
+      </c>
+      <c r="E37" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>51</v>
       </c>
@@ -1194,11 +1268,14 @@
       <c r="C38" s="7">
         <v>0.1016</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="14">
+        <v>4113809</v>
+      </c>
+      <c r="E38" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>51</v>
       </c>
@@ -1206,8 +1283,11 @@
         <v>2021</v>
       </c>
       <c r="C39" s="7"/>
-    </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D39" s="14">
+        <v>4113809</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>51</v>
       </c>
@@ -1217,14 +1297,18 @@
       <c r="C40" s="7">
         <v>4.48E-2</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="14">
+        <v>4113809</v>
+      </c>
+      <c r="E40" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C41" s="7"/>
-    </row>
-    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D41" s="14"/>
+    </row>
+    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>50</v>
       </c>
@@ -1234,11 +1318,14 @@
       <c r="C42" s="7">
         <v>0.05</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="14">
+        <v>4111902</v>
+      </c>
+      <c r="E42" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>50</v>
       </c>
@@ -1248,11 +1335,14 @@
       <c r="C43" s="7">
         <v>0.05</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="14">
+        <v>4111902</v>
+      </c>
+      <c r="E43" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>50</v>
       </c>
@@ -1262,11 +1352,14 @@
       <c r="C44" s="7">
         <v>0.14949999999999999</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="14">
+        <v>4111902</v>
+      </c>
+      <c r="E44" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>50</v>
       </c>
@@ -1276,11 +1369,14 @@
       <c r="C45" s="7">
         <v>0.15</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="14">
+        <v>4111902</v>
+      </c>
+      <c r="E45" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>50</v>
       </c>
@@ -1290,11 +1386,14 @@
       <c r="C46" s="7">
         <v>5.5300000000000002E-2</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="14">
+        <v>4111902</v>
+      </c>
+      <c r="E46" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>50</v>
       </c>
@@ -1304,14 +1403,18 @@
       <c r="C47" s="7">
         <v>2.2499999999999999E-2</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="14">
+        <v>4111902</v>
+      </c>
+      <c r="E47" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C48" s="7"/>
-    </row>
-    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D48" s="14"/>
+    </row>
+    <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>43</v>
       </c>
@@ -1321,11 +1424,14 @@
       <c r="C49" s="7">
         <v>4.8300000000000003E-2</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="14">
+        <v>4120507</v>
+      </c>
+      <c r="E49" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>43</v>
       </c>
@@ -1335,11 +1441,14 @@
       <c r="C50" s="7">
         <v>0.11460000000000001</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="14">
+        <v>4120507</v>
+      </c>
+      <c r="E50" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>43</v>
       </c>
@@ -1349,11 +1458,14 @@
       <c r="C51" s="7">
         <v>0.1263</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D51" s="14">
+        <v>4120507</v>
+      </c>
+      <c r="E51" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>43</v>
       </c>
@@ -1363,11 +1475,14 @@
       <c r="C52" s="7">
         <v>0.15</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D52" s="14">
+        <v>4120507</v>
+      </c>
+      <c r="E52" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>43</v>
       </c>
@@ -1377,11 +1492,14 @@
       <c r="C53" s="7">
         <v>4.5199999999999997E-2</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="14">
+        <v>4120507</v>
+      </c>
+      <c r="E53" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>43</v>
       </c>
@@ -1391,56 +1509,65 @@
       <c r="C54" s="7">
         <v>7.3178999999999994E-2</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D54" s="14">
+        <v>4120507</v>
+      </c>
+      <c r="E54" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D55" s="14"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D56" s="14"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C63" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E13" r:id="rId1" xr:uid="{EE75B64B-C7A6-44B4-8AC6-F3C7CDC64C71}"/>
-    <hyperlink ref="E15" r:id="rId2" xr:uid="{C38C7F79-A64F-4623-BD4F-580F8AFD061E}"/>
-    <hyperlink ref="E16" r:id="rId3" xr:uid="{E0055D9C-CACE-40E3-912F-7552840A1BCA}"/>
-    <hyperlink ref="E17" r:id="rId4" xr:uid="{4144CF7D-4FBF-496C-B5BA-D32D7B91A82A}"/>
-    <hyperlink ref="E3" r:id="rId5" xr:uid="{CD081003-8374-428A-B2F7-D9DAE84025E1}"/>
-    <hyperlink ref="E5" r:id="rId6" xr:uid="{DF98840A-BED1-49E1-B92D-46CC476DBA26}"/>
-    <hyperlink ref="E6" r:id="rId7" xr:uid="{2035362C-9A91-4B81-829D-3D0C4FA771DF}"/>
-    <hyperlink ref="E14" r:id="rId8" xr:uid="{CE999FD0-8CBC-4BEA-84BE-95B4E1C3A1C5}"/>
-    <hyperlink ref="D22" r:id="rId9" display="https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2023/609/lei-ordinaria-n-609-2023-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias" xr:uid="{C3275B82-C56D-4C85-BA27-2F2BD690BB16}"/>
-    <hyperlink ref="D20" r:id="rId10" display="https://leis.org/municipais/pr/cafeara/lei/lei-complementar/2025/669/lei-complementar-n-669-2025-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL" xr:uid="{A7EAD4F8-68E0-41D4-AE50-5A0B782E8B8F}"/>
-    <hyperlink ref="D21" r:id="rId11" display="https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2024/636/lei-ordinaria-n-636-2024-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL" xr:uid="{23D66F80-65EE-4A0F-8144-F36DB20450EF}"/>
-    <hyperlink ref="D23" r:id="rId12" display="https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2022/587/lei-ordinaria-n-587-2022-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL" xr:uid="{1B38F967-CA98-456B-9E39-53D8B29C2593}"/>
-    <hyperlink ref="D24" r:id="rId13" display="https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2021/563/lei-ordinaria-n-563-2021-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL" xr:uid="{2F2E9EFC-04E5-4D6C-ADAE-3D1C1FE4D8C2}"/>
-    <hyperlink ref="D25" r:id="rId14" display="https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2020/542/lei-ordinaria-n-542-2020-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-revisao-salarial-aos-servidores-publicos-municipais-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL" xr:uid="{CE150FB9-81B7-4D95-A8CF-6EF4FEC69817}"/>
-    <hyperlink ref="D27" r:id="rId15" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2025/325/3248/lei-ordinaria-n-3248-2025-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-com-excecao-dos-subsidios-dos-agentes-politicos?q=reajuste" xr:uid="{14532045-718C-41E1-8B54-50EFD37FBDB7}"/>
-    <hyperlink ref="D28" r:id="rId16" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2024/322/3211/lei-ordinaria-n-3211-2024-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-inclusive-sobre-os-subsidios-dos-agentes-politicos?q=reajuste" xr:uid="{38AE6B04-78B2-4EB9-9571-DB2D521C73B5}"/>
-    <hyperlink ref="D29" r:id="rId17" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2023/317/3170/lei-ordinaria-n-3170-2023-autoriza-a-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-inclusive-sobre-os-subsidios-dos-agentes-politicos?q=reajuste" xr:uid="{4CF69429-E3A8-42D6-85E9-C1B4DF636DEA}"/>
-    <hyperlink ref="D30" r:id="rId18" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2022/314/3132/lei-ordinaria-n-3132-2022-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-inclusive-sobre-os-subsidios-dos-agentes-politicos?q=reajuste" xr:uid="{55BFE9D4-B84C-4424-B8D7-86FC64A9AB3E}"/>
-    <hyperlink ref="D31" r:id="rId19" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2021/310/3097/lei-ordinaria-n-3097-2021-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao?q=reajuste" xr:uid="{87876156-98C2-4000-91CE-7C8AD0B3476E}"/>
-    <hyperlink ref="D32" r:id="rId20" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2020/305/3045/lei-ordinaria-n-3045-2020-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-inclusive-sobre-os-subsidios-dos-agentes-politicos-bem-como-adequa-o-salario-dos-servidores-do-quadro-do-magisterio-publico-municipal-ao-piso-salarial-profissional-nacional?q=reajuste" xr:uid="{DF65B76A-65AA-4C35-A537-F477C0AB6BF4}"/>
-    <hyperlink ref="E18" r:id="rId21" xr:uid="{EC4616F6-7680-425A-9B5B-FA1377623831}"/>
-    <hyperlink ref="D10" r:id="rId22" xr:uid="{5B0B0D6A-84BF-4334-B8E3-04EFE33A5016}"/>
-    <hyperlink ref="D2" r:id="rId23" xr:uid="{5300EFF3-C77D-4044-9FEE-10FEE221CCA5}"/>
-    <hyperlink ref="D34" r:id="rId24" xr:uid="{0198FF07-6ABC-4FE0-BC94-9626A092EF1E}"/>
-    <hyperlink ref="D35" r:id="rId25" xr:uid="{9B9DADFC-147D-439F-A89B-8D7EC2EFFA45}"/>
-    <hyperlink ref="D36" r:id="rId26" xr:uid="{7B4312A5-B4D6-48C3-9967-D4A547A0F189}"/>
-    <hyperlink ref="D40" r:id="rId27" xr:uid="{B555F1DF-7AE0-4CE3-A746-A72DB71A3814}"/>
-    <hyperlink ref="D42" r:id="rId28" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2025/1/3/lei-ordinaria-n-3-2025-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{79AF655C-919A-4B59-8D63-6E9B71A0DFD8}"/>
-    <hyperlink ref="D43" r:id="rId29" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2024/1/6/lei-ordinaria-n-6-2024-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-e-recomposicao-inflacionaria-aos-agentes-politicos-do-poder-executivo-prefeito-vice-prefeito-e-secretarios-municipais-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{28DF2AEC-02FD-4904-92E4-8F1A46B7C53A}"/>
-    <hyperlink ref="D44" r:id="rId30" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2023/1/3/lei-ordinaria-n-3-2023-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-e-recomposicao-inflacionaria-aos-agentes-politicos-do-poder-executivo-prefeito-vice-prefeito-e-secretarios-municipais-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{D52BDBF7-13A5-4A80-A127-116B587657FB}"/>
-    <hyperlink ref="D45" r:id="rId31" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2022/1/5/lei-ordinaria-n-5-2022-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{3E75ABFE-1194-4B2F-AF68-D20DEC412ED8}"/>
-    <hyperlink ref="D46" r:id="rId32" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2021/1/5/lei-ordinaria-n-5-2021-concede-recomposicao-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{4FC8FEEE-0401-4369-8921-ED4B51F5562D}"/>
-    <hyperlink ref="D47" r:id="rId33" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2020/2/11/lei-ordinaria-n-11-2020-concede-recomposicao-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-e-ao-prefeito-vice-prefeito-e-secretarios-municipais-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{4D8E764E-22B9-4B1F-A195-598C7E088B03}"/>
-    <hyperlink ref="D51" r:id="rId34" xr:uid="{469628B4-8B6D-46C9-A62E-832B5D06C62E}"/>
-    <hyperlink ref="D54" r:id="rId35" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2020/74/739/lei-ordinaria-n-739-2020-dispoe-sobre-a-revisao-geral-anual-do-subsidio-do-prefeito-vice-prefeito-vereadores-secretarios-as-municipais-e-remuneracao-do-s-servidor-es-comissionados-e-estatutario-do-poder-legislativo-do-municipio-de-primeiro-de-maio-e-da-outras-providencias?q=salarial%20" xr:uid="{8F367E47-ABB7-4AAB-A611-4BB40BDA61A3}"/>
-    <hyperlink ref="D49" r:id="rId36" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2025/97/970/lei-ordinaria-n-970-2025-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{9C1E9D0B-D3E4-4ECB-928C-3AB9384788C0}"/>
-    <hyperlink ref="D50" r:id="rId37" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2024/94/934/lei-ordinaria-n-934-2024-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{AF964D4D-7701-48C8-898F-A6225D73AC79}"/>
-    <hyperlink ref="D52" r:id="rId38" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2022/80/800/lei-ordinaria-n-800-2022-dispoe-sobre-a-revisao-geral-anual-do-subsidio-do-prefeito-vice-prefeito-vereadores-secretarios-as-municipais-e-remuneracao-do-s-servidor-es-comissionados-e-estatutario-do-poder-legislativo-do-municipio-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{98F545B3-8D3D-44B1-AB35-4AC2759963EB}"/>
-    <hyperlink ref="D53" r:id="rId39" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2021/77/770/lei-ordinaria-n-770-2021-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{C52DDB23-FB88-489B-BD74-E79A0801ADF5}"/>
-    <hyperlink ref="D38" r:id="rId40" xr:uid="{878A7E66-55B4-4DAF-8A75-A1CF624BBEC7}"/>
-    <hyperlink ref="D37" r:id="rId41" xr:uid="{47F34AB3-0A0A-412F-8FE1-03EF5CACC9CA}"/>
+    <hyperlink ref="F13" r:id="rId1" xr:uid="{EE75B64B-C7A6-44B4-8AC6-F3C7CDC64C71}"/>
+    <hyperlink ref="F15" r:id="rId2" xr:uid="{C38C7F79-A64F-4623-BD4F-580F8AFD061E}"/>
+    <hyperlink ref="F16" r:id="rId3" xr:uid="{E0055D9C-CACE-40E3-912F-7552840A1BCA}"/>
+    <hyperlink ref="F17" r:id="rId4" xr:uid="{4144CF7D-4FBF-496C-B5BA-D32D7B91A82A}"/>
+    <hyperlink ref="F3" r:id="rId5" xr:uid="{CD081003-8374-428A-B2F7-D9DAE84025E1}"/>
+    <hyperlink ref="F5" r:id="rId6" xr:uid="{DF98840A-BED1-49E1-B92D-46CC476DBA26}"/>
+    <hyperlink ref="F6" r:id="rId7" xr:uid="{2035362C-9A91-4B81-829D-3D0C4FA771DF}"/>
+    <hyperlink ref="F14" r:id="rId8" xr:uid="{CE999FD0-8CBC-4BEA-84BE-95B4E1C3A1C5}"/>
+    <hyperlink ref="E22" r:id="rId9" display="https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2023/609/lei-ordinaria-n-609-2023-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias" xr:uid="{C3275B82-C56D-4C85-BA27-2F2BD690BB16}"/>
+    <hyperlink ref="E20" r:id="rId10" display="https://leis.org/municipais/pr/cafeara/lei/lei-complementar/2025/669/lei-complementar-n-669-2025-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL" xr:uid="{A7EAD4F8-68E0-41D4-AE50-5A0B782E8B8F}"/>
+    <hyperlink ref="E21" r:id="rId11" display="https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2024/636/lei-ordinaria-n-636-2024-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL" xr:uid="{23D66F80-65EE-4A0F-8144-F36DB20450EF}"/>
+    <hyperlink ref="E23" r:id="rId12" display="https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2022/587/lei-ordinaria-n-587-2022-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL" xr:uid="{1B38F967-CA98-456B-9E39-53D8B29C2593}"/>
+    <hyperlink ref="E24" r:id="rId13" display="https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2021/563/lei-ordinaria-n-563-2021-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL" xr:uid="{2F2E9EFC-04E5-4D6C-ADAE-3D1C1FE4D8C2}"/>
+    <hyperlink ref="E25" r:id="rId14" display="https://leis.org/municipais/pr/cafeara/lei/lei-ordinaria/2020/542/lei-ordinaria-n-542-2020-autoriza-o-executivo-municipal-a-conceder-recomposicao-geral-anual-aos-servidores-publicos-municipais-e-agentes-politicos-do-poder-executivo-municipal-de-cafeara-e-revisao-salarial-aos-servidores-publicos-municipais-e-da-outras-providencias?termo=RECOMPOSI%C3%87%C3%83O%20GERAL%20ANUAL" xr:uid="{CE150FB9-81B7-4D95-A8CF-6EF4FEC69817}"/>
+    <hyperlink ref="E27" r:id="rId15" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2025/325/3248/lei-ordinaria-n-3248-2025-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-com-excecao-dos-subsidios-dos-agentes-politicos?q=reajuste" xr:uid="{14532045-718C-41E1-8B54-50EFD37FBDB7}"/>
+    <hyperlink ref="E28" r:id="rId16" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2024/322/3211/lei-ordinaria-n-3211-2024-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-inclusive-sobre-os-subsidios-dos-agentes-politicos?q=reajuste" xr:uid="{38AE6B04-78B2-4EB9-9571-DB2D521C73B5}"/>
+    <hyperlink ref="E29" r:id="rId17" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2023/317/3170/lei-ordinaria-n-3170-2023-autoriza-a-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-inclusive-sobre-os-subsidios-dos-agentes-politicos?q=reajuste" xr:uid="{4CF69429-E3A8-42D6-85E9-C1B4DF636DEA}"/>
+    <hyperlink ref="E30" r:id="rId18" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2022/314/3132/lei-ordinaria-n-3132-2022-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-inclusive-sobre-os-subsidios-dos-agentes-politicos?q=reajuste" xr:uid="{55BFE9D4-B84C-4424-B8D7-86FC64A9AB3E}"/>
+    <hyperlink ref="E31" r:id="rId19" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2021/310/3097/lei-ordinaria-n-3097-2021-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao?q=reajuste" xr:uid="{87876156-98C2-4000-91CE-7C8AD0B3476E}"/>
+    <hyperlink ref="E32" r:id="rId20" display="https://leismunicipais.com.br/a1/pr/c/centenario-do-sul/lei-ordinaria/2020/305/3045/lei-ordinaria-n-3045-2020-autoriza-o-chefe-do-poder-executivo-municipal-a-conceder-reposicao-salarial-nos-vencimentos-e-proventos-dos-servidores-ativos-inativos-e-pensionistas-efetivo-ou-em-comissao-inclusive-sobre-os-subsidios-dos-agentes-politicos-bem-como-adequa-o-salario-dos-servidores-do-quadro-do-magisterio-publico-municipal-ao-piso-salarial-profissional-nacional?q=reajuste" xr:uid="{DF65B76A-65AA-4C35-A537-F477C0AB6BF4}"/>
+    <hyperlink ref="F18" r:id="rId21" xr:uid="{EC4616F6-7680-425A-9B5B-FA1377623831}"/>
+    <hyperlink ref="E10" r:id="rId22" xr:uid="{5B0B0D6A-84BF-4334-B8E3-04EFE33A5016}"/>
+    <hyperlink ref="E2" r:id="rId23" xr:uid="{5300EFF3-C77D-4044-9FEE-10FEE221CCA5}"/>
+    <hyperlink ref="E34" r:id="rId24" xr:uid="{0198FF07-6ABC-4FE0-BC94-9626A092EF1E}"/>
+    <hyperlink ref="E35" r:id="rId25" xr:uid="{9B9DADFC-147D-439F-A89B-8D7EC2EFFA45}"/>
+    <hyperlink ref="E36" r:id="rId26" xr:uid="{7B4312A5-B4D6-48C3-9967-D4A547A0F189}"/>
+    <hyperlink ref="E40" r:id="rId27" xr:uid="{B555F1DF-7AE0-4CE3-A746-A72DB71A3814}"/>
+    <hyperlink ref="E42" r:id="rId28" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2025/1/3/lei-ordinaria-n-3-2025-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{79AF655C-919A-4B59-8D63-6E9B71A0DFD8}"/>
+    <hyperlink ref="E43" r:id="rId29" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2024/1/6/lei-ordinaria-n-6-2024-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-e-recomposicao-inflacionaria-aos-agentes-politicos-do-poder-executivo-prefeito-vice-prefeito-e-secretarios-municipais-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{28DF2AEC-02FD-4904-92E4-8F1A46B7C53A}"/>
+    <hyperlink ref="E44" r:id="rId30" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2023/1/3/lei-ordinaria-n-3-2023-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-e-recomposicao-inflacionaria-aos-agentes-politicos-do-poder-executivo-prefeito-vice-prefeito-e-secretarios-municipais-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{D52BDBF7-13A5-4A80-A127-116B587657FB}"/>
+    <hyperlink ref="E45" r:id="rId31" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2022/1/5/lei-ordinaria-n-5-2022-concede-recomposicao-e-reajuste-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{3E75ABFE-1194-4B2F-AF68-D20DEC412ED8}"/>
+    <hyperlink ref="E46" r:id="rId32" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2021/1/5/lei-ordinaria-n-5-2021-concede-recomposicao-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{4FC8FEEE-0401-4369-8921-ED4B51F5562D}"/>
+    <hyperlink ref="E47" r:id="rId33" display="https://leismunicipais.com.br/a/pr/j/jaguapita/lei-ordinaria/2020/2/11/lei-ordinaria-n-11-2020-concede-recomposicao-salarial-aos-servidores-da-administracao-direta-e-indireta-do-poder-executivo-e-ao-prefeito-vice-prefeito-e-secretarios-municipais-desta-municipalidade-nos-termos-do-artigo-37-x-da-constituicao-federal-e-da-outras-providencias?q=recomposi%E7%E3o%20salarial" xr:uid="{4D8E764E-22B9-4B1F-A195-598C7E088B03}"/>
+    <hyperlink ref="E51" r:id="rId34" xr:uid="{469628B4-8B6D-46C9-A62E-832B5D06C62E}"/>
+    <hyperlink ref="E54" r:id="rId35" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2020/74/739/lei-ordinaria-n-739-2020-dispoe-sobre-a-revisao-geral-anual-do-subsidio-do-prefeito-vice-prefeito-vereadores-secretarios-as-municipais-e-remuneracao-do-s-servidor-es-comissionados-e-estatutario-do-poder-legislativo-do-municipio-de-primeiro-de-maio-e-da-outras-providencias?q=salarial%20" xr:uid="{8F367E47-ABB7-4AAB-A611-4BB40BDA61A3}"/>
+    <hyperlink ref="E49" r:id="rId36" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2025/97/970/lei-ordinaria-n-970-2025-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{9C1E9D0B-D3E4-4ECB-928C-3AB9384788C0}"/>
+    <hyperlink ref="E50" r:id="rId37" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2024/94/934/lei-ordinaria-n-934-2024-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{AF964D4D-7701-48C8-898F-A6225D73AC79}"/>
+    <hyperlink ref="E52" r:id="rId38" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2022/80/800/lei-ordinaria-n-800-2022-dispoe-sobre-a-revisao-geral-anual-do-subsidio-do-prefeito-vice-prefeito-vereadores-secretarios-as-municipais-e-remuneracao-do-s-servidor-es-comissionados-e-estatutario-do-poder-legislativo-do-municipio-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{98F545B3-8D3D-44B1-AB35-4AC2759963EB}"/>
+    <hyperlink ref="E53" r:id="rId39" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2021/77/770/lei-ordinaria-n-770-2021-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{C52DDB23-FB88-489B-BD74-E79A0801ADF5}"/>
+    <hyperlink ref="E38" r:id="rId40" xr:uid="{878A7E66-55B4-4DAF-8A75-A1CF624BBEC7}"/>
+    <hyperlink ref="E37" r:id="rId41" xr:uid="{47F34AB3-0A0A-412F-8FE1-03EF5CACC9CA}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId42"/>
@@ -1449,18 +1576,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD7E18E-7E3E-4609-9E74-70EF657891A1}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>54</v>
       </c>
@@ -1470,11 +1598,14 @@
       <c r="C1" s="7">
         <v>4.8300000000000003E-2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="14">
+        <v>4120333</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>54</v>
       </c>
@@ -1484,11 +1615,14 @@
       <c r="C2" s="7">
         <v>4.6199999999999998E-2</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="14">
+        <v>4120333</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>54</v>
       </c>
@@ -1498,11 +1632,14 @@
       <c r="C3" s="7">
         <v>5.9299999999999999E-2</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="14">
+        <v>4120333</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>54</v>
       </c>
@@ -1512,11 +1649,14 @@
       <c r="C4" s="7">
         <v>0.1</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="14">
+        <v>4120333</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>54</v>
       </c>
@@ -1526,11 +1666,14 @@
       <c r="C5" s="7">
         <v>4.5199999999999997E-2</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="14">
+        <v>4120333</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>54</v>
       </c>
@@ -1540,15 +1683,19 @@
       <c r="C6" s="7">
         <v>4.3099999999999999E-2</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="14">
+        <v>4120333</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="14"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>61</v>
       </c>
@@ -1558,8 +1705,11 @@
       <c r="C8" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="14">
+        <v>4109203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>61</v>
       </c>
@@ -1569,8 +1719,11 @@
       <c r="C9" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="14">
+        <v>4109203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>61</v>
       </c>
@@ -1580,8 +1733,11 @@
       <c r="C10" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="14">
+        <v>4109203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>61</v>
       </c>
@@ -1591,8 +1747,11 @@
       <c r="C11" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="14">
+        <v>4109203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>61</v>
       </c>
@@ -1602,8 +1761,11 @@
       <c r="C12" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="14">
+        <v>4109203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>61</v>
       </c>
@@ -1613,8 +1775,14 @@
       <c r="C13" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="14">
+        <v>4109203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="14"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>62</v>
       </c>
@@ -1624,8 +1792,11 @@
       <c r="C15" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="14">
+        <v>4120002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>62</v>
       </c>
@@ -1635,8 +1806,11 @@
       <c r="C16" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="14">
+        <v>4120002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>62</v>
       </c>
@@ -1646,8 +1820,11 @@
       <c r="C17" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="14">
+        <v>4120002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>62</v>
       </c>
@@ -1657,8 +1834,11 @@
       <c r="C18" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="14">
+        <v>4120002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>62</v>
       </c>
@@ -1668,8 +1848,11 @@
       <c r="C19" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="14">
+        <v>4120002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>62</v>
       </c>
@@ -1679,10 +1862,16 @@
       <c r="C20" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="14">
+        <v>4120002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="14"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B22" s="5">
         <v>2025</v>
@@ -1690,10 +1879,13 @@
       <c r="C22" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="14">
+        <v>4108007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B23" s="5">
         <v>2024</v>
@@ -1701,10 +1893,13 @@
       <c r="C23" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="14">
+        <v>4108007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B24" s="5">
         <v>2023</v>
@@ -1712,10 +1907,13 @@
       <c r="C24" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="14">
+        <v>4108007</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B25" s="5">
         <v>2022</v>
@@ -1723,10 +1921,13 @@
       <c r="C25" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="14">
+        <v>4108007</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B26" s="5">
         <v>2021</v>
@@ -1734,10 +1935,13 @@
       <c r="C26" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="14">
+        <v>4108007</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B27" s="5">
         <v>2020</v>
@@ -1745,15 +1949,18 @@
       <c r="C27" s="7">
         <v>0</v>
       </c>
+      <c r="D27" s="14">
+        <v>4108007</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-complementar/2022/59/583/lei-complementar-n-583-2022-dispoe-sobre-aumento-salarial-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=aumento%20salarial" xr:uid="{7A2912B1-A033-4B0B-8FE9-0051BC578F1E}"/>
-    <hyperlink ref="D1" r:id="rId2" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2025/63/630/lei-ordinaria-n-630-2025-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{C25B9C11-3CAB-45EA-8DAC-5798EA66F1FB}"/>
-    <hyperlink ref="D2" r:id="rId3" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2024/62/614/lei-ordinaria-n-614-2024-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{180B63DB-B3CA-4BE9-BE93-A756811226FC}"/>
-    <hyperlink ref="D3" r:id="rId4" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2023/59/588/lei-ordinaria-n-588-2023-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{27C5E00F-A21E-4F3D-B440-EEA8732A0606}"/>
-    <hyperlink ref="D5" r:id="rId5" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2021/54/534/lei-ordinaria-n-534-2021-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{A8A960AF-CE07-462C-818F-7309432BE808}"/>
-    <hyperlink ref="D6" r:id="rId6" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2020/52/516/lei-ordinaria-n-516-2020-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{65B1BDEA-E442-424A-AFC9-2BF060B58188}"/>
+    <hyperlink ref="E4" r:id="rId1" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-complementar/2022/59/583/lei-complementar-n-583-2022-dispoe-sobre-aumento-salarial-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=aumento%20salarial" xr:uid="{7A2912B1-A033-4B0B-8FE9-0051BC578F1E}"/>
+    <hyperlink ref="E1" r:id="rId2" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2025/63/630/lei-ordinaria-n-630-2025-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{C25B9C11-3CAB-45EA-8DAC-5798EA66F1FB}"/>
+    <hyperlink ref="E2" r:id="rId3" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2024/62/614/lei-ordinaria-n-614-2024-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{180B63DB-B3CA-4BE9-BE93-A756811226FC}"/>
+    <hyperlink ref="E3" r:id="rId4" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2023/59/588/lei-ordinaria-n-588-2023-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{27C5E00F-A21E-4F3D-B440-EEA8732A0606}"/>
+    <hyperlink ref="E5" r:id="rId5" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2021/54/534/lei-ordinaria-n-534-2021-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{A8A960AF-CE07-462C-818F-7309432BE808}"/>
+    <hyperlink ref="E6" r:id="rId6" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2020/52/516/lei-ordinaria-n-516-2020-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{65B1BDEA-E442-424A-AFC9-2BF060B58188}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
addeds  santa fe  e prado
</commit_message>
<xml_diff>
--- a/data/dados.xlsx
+++ b/data/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\reajuste\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1424D274-2029-4EF0-9A99-C154FED1D0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36AEF93-4DAC-4AD4-BE46-53EC55C541CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="1" xr2:uid="{BE2A1F3B-6535-41F1-9783-CEB15E5262F6}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{BE2A1F3B-6535-41F1-9783-CEB15E5262F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="79">
   <si>
     <t>Cafeara</t>
   </si>
@@ -232,6 +232,48 @@
   </si>
   <si>
     <t>Florestópolis</t>
+  </si>
+  <si>
+    <t>https://leismunicipais.com.br/a1/pr/p/porecatu/lei-ordinaria/2022/193/1928/lei-ordinaria-n-1928-2022-dispoe-sobre-a-reposicao-salarial-dos-cargos-pertencentes-ao-quadro-proprio-de-servidores-publicos-do-municipio-de-porecatu-inclusive-inativos-e-pensionistas-e-dos-subsidios-dos-secretarios-municipais-prefeito-e-vice-prefeito-e-da-outras-providencias?q=reajuste</t>
+  </si>
+  <si>
+    <t>https://leismunicipais.com.br/a1/pr/p/porecatu/lei-ordinaria/2024/200/1991/lei-ordinaria-n-1991-2024-concede-a-reposicao-de-perdas-salariais-aos-servidores-ativos-e-inativos-e-aos-vereadores-do-poder-legislativo-da-camara-municipal-de-porecatu-e-da-outras-proviencias?q=REPOSI%C7%C3O%20SALARIAL</t>
+  </si>
+  <si>
+    <t>https://leismunicipais.com.br/a1/pr/p/porecatu/lei-ordinaria/2023/198/1971/lei-ordinaria-n-1971-2023-dispoe-sobre-a-reposicao-salarial-dos-cargos-pertencentes-ao-quadro-proprio-de-servidores-publicos-do-municipio-de-porecatu-inclusive-inativos-e-pensionistas-e-dos-subsidios-dos-secretarios-municipais-e-da-outras-providencias?q=REPOSI%C7%C3O%20SALARIAL</t>
+  </si>
+  <si>
+    <t>https://leismunicipais.com.br/a1/pr/p/porecatu/lei-ordinaria/2021/190/1893/lei-ordinaria-n-1893-2021-dispoe-sobre-a-reposicao-salarial-dos-cargos-pertencentes-ao-quadro-proprio-de-servidores-publicos-do-municipio-de-porecatu-inclusive-inativos-e-pensionistas-e-dos-subsidios-dos-secretarios-municipais-e-da-outras-providencias?q=REPOSI%C7%C3O%20SALARIAL</t>
+  </si>
+  <si>
+    <t>https://leismunicipais.com.br/a1/pr/p/porecatu/lei-ordinaria/2020/186/1857/lei-ordinaria-n-1857-2020-dispoe-sobre-a-reposicao-salarial-dos-cargos-pertencentes-ao-quadro-proprio-de-servidores-publicos-do-municipio-de-porecatu-inclusive-inativos-e-pensionistas-e-dos-subsidios-dos-secretarios-municipais-e-da-outras-providencias?q=REPOSI%C7%C3O%20SALARIAL</t>
+  </si>
+  <si>
+    <t>Santa Fé</t>
+  </si>
+  <si>
+    <t>https://santafe.oxy.elotech.com.br/portaltransparencia-api/api/files/arquivo/326310</t>
+  </si>
+  <si>
+    <t>https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2024/232/2320/lei-ordinaria-n-2320-2024-autoriza-revisao-geral-da-remuneracao-e-os-subsidios-dos-servidores-publicos-e-agentes-politicos-dos-poderes-executivo-e-legislativo-do-municipio-nos-termos-do-artigo-7-caput-iv-e-o-do-artigo-39-3-da-constituicao-federal-extensivo-aos-conselheiros-tutelares-e-aos-proventos-dos-inativos-e-pensionistas?q=Revis%C3%A3o+geraL</t>
+  </si>
+  <si>
+    <t>laude.ai/oauth/authorize?code=true&amp;client_id=9d1c250a-e61b-44d9-88ed-5944d1962f5e&amp;response_type=code&amp;scope=user%3Ainference+user%3Aprofile&amp;code_challenge=VB2R7iclQx47HBmFnLOpMyyTRW2SmHbvR14eAKSZZC0&amp;code_challenge_method=S256&amp;state=0E12of1whNvA7TAf0HAlrRXhuXtorucbwznvGvr1NFA&amp;redirect_uri=https%3A%2F%2Fconsole.anthropic.com%2Foauth%2Fcode%2Fcallback</t>
+  </si>
+  <si>
+    <t>https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2021/218/2180/lei-ordinaria-n-2180-2021-suspende-os-efeitos-da-lei-municipal-n-2147-2021-que-autoriza-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-e-da-outras-providencias?q=Revis%E3o%20geraL</t>
+  </si>
+  <si>
+    <t>https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2020/211/2107/lei-ordinaria-n-2107-2020-autoriza-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-a-aplicacao-do-artigo-7-inciso-iv-e-art-39-3-da-constituicao-federal-a-remuneracao-dos-servidores-publicos-o-reajuste-dos-proventos-dos-inativos-e-pensionistas-a-recomposicao-dos-subsidios-dos-agentes-politicos-e-fixa-os-pisos-nacionais-minimos-para-os-integrantes-do-magisterio-municipal-11739-2008-e-da-outras-providencias?q=Revis%E3o%20geraL</t>
+  </si>
+  <si>
+    <t>https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2021/220/2198/lei-ordinaria-n-2198-2021-autoriza-revisao-geral-da-remuneracao-dos-servidores-publicos-autoriza-a-aplicacao-do-artigo-7-caput-iv-e-o-do-artigo-39-3-da-constituicao-federal-a-remuneracao-dos-servidores-publicos-e-autoriza-o-reajuste-dos-proventos-dos-inativos-e-pensionistas?q=2.198</t>
+  </si>
+  <si>
+    <t>https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2021/220/2197/lei-ordinaria-n-2197-2021-autoriza-revisao-geral-da-remuneracao-dos-servidores-publicos-autoriza-a-aplicacao-do-artigo-7-caput-iv-e-o-do-artigo-39-3-da-constituicao-federal-a-remuneracao-dos-servidores-publicos-e-autoriza-o-reajuste-dos-proventos-dos-inativos-e-pensionistas?q=2.197</t>
+  </si>
+  <si>
+    <t>Miraselva</t>
   </si>
 </sst>
 </file>
@@ -289,12 +331,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -310,7 +358,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -340,6 +388,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -677,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A9F774-A2B7-43E0-89BB-A01627A8B05C}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D23:D24"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -714,7 +770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
@@ -725,7 +781,7 @@
         <v>4.2599999999999999E-2</v>
       </c>
       <c r="D2" s="12"/>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F2" s="1"/>
@@ -837,7 +893,7 @@
       <c r="C10" s="7">
         <v>6.7900000000000002E-2</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="8"/>
@@ -990,7 +1046,7 @@
       <c r="D20" s="14">
         <v>4103404</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1007,7 +1063,7 @@
       <c r="D21" s="14">
         <v>4103404</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1024,7 +1080,7 @@
       <c r="D22" s="14">
         <v>4103404</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1041,7 +1097,7 @@
       <c r="D23" s="14">
         <v>4103404</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1058,7 +1114,7 @@
       <c r="D24" s="14">
         <v>4103404</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1075,7 +1131,7 @@
       <c r="D25" s="14">
         <v>4103404</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1083,7 +1139,7 @@
       <c r="C26" s="7"/>
       <c r="D26" s="14"/>
     </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>52</v>
       </c>
@@ -1096,11 +1152,11 @@
       <c r="D27" s="14">
         <v>4105102</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>52</v>
       </c>
@@ -1113,11 +1169,11 @@
       <c r="D28" s="14">
         <v>4105102</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>52</v>
       </c>
@@ -1130,11 +1186,11 @@
       <c r="D29" s="14">
         <v>4105102</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>52</v>
       </c>
@@ -1147,11 +1203,11 @@
       <c r="D30" s="14">
         <v>4105102</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>52</v>
       </c>
@@ -1164,11 +1220,11 @@
       <c r="D31" s="14">
         <v>4105102</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>52</v>
       </c>
@@ -1181,16 +1237,15 @@
       <c r="D32" s="14">
         <v>4105102</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C33" s="7"/>
       <c r="D33" s="14"/>
-      <c r="E33" s="8"/>
-    </row>
-    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>51</v>
       </c>
@@ -1203,11 +1258,11 @@
       <c r="D34" s="14">
         <v>4113809</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>51</v>
       </c>
@@ -1220,11 +1275,11 @@
       <c r="D35" s="14">
         <v>4113809</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>51</v>
       </c>
@@ -1237,11 +1292,11 @@
       <c r="D36" s="14">
         <v>4113809</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>51</v>
       </c>
@@ -1254,11 +1309,11 @@
       <c r="D37" s="14">
         <v>4113809</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>51</v>
       </c>
@@ -1271,7 +1326,7 @@
       <c r="D38" s="14">
         <v>4113809</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1287,7 +1342,7 @@
         <v>4113809</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>51</v>
       </c>
@@ -1300,7 +1355,7 @@
       <c r="D40" s="14">
         <v>4113809</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E40" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1308,7 +1363,7 @@
       <c r="C41" s="7"/>
       <c r="D41" s="14"/>
     </row>
-    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>50</v>
       </c>
@@ -1321,11 +1376,11 @@
       <c r="D42" s="14">
         <v>4111902</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>50</v>
       </c>
@@ -1338,11 +1393,11 @@
       <c r="D43" s="14">
         <v>4111902</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="E43" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>50</v>
       </c>
@@ -1355,11 +1410,11 @@
       <c r="D44" s="14">
         <v>4111902</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="E44" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>50</v>
       </c>
@@ -1372,11 +1427,11 @@
       <c r="D45" s="14">
         <v>4111902</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E45" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>50</v>
       </c>
@@ -1389,11 +1444,11 @@
       <c r="D46" s="14">
         <v>4111902</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="E46" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>50</v>
       </c>
@@ -1406,7 +1461,7 @@
       <c r="D47" s="14">
         <v>4111902</v>
       </c>
-      <c r="E47" s="8" t="s">
+      <c r="E47" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1414,7 +1469,7 @@
       <c r="C48" s="7"/>
       <c r="D48" s="14"/>
     </row>
-    <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>43</v>
       </c>
@@ -1427,11 +1482,11 @@
       <c r="D49" s="14">
         <v>4120507</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="E49" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>43</v>
       </c>
@@ -1444,11 +1499,11 @@
       <c r="D50" s="14">
         <v>4120507</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="E50" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>43</v>
       </c>
@@ -1461,11 +1516,11 @@
       <c r="D51" s="14">
         <v>4120507</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="E51" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>43</v>
       </c>
@@ -1478,11 +1533,11 @@
       <c r="D52" s="14">
         <v>4120507</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E52" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>43</v>
       </c>
@@ -1495,11 +1550,11 @@
       <c r="D53" s="14">
         <v>4120507</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E53" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>43</v>
       </c>
@@ -1512,7 +1567,7 @@
       <c r="D54" s="14">
         <v>4120507</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="E54" s="3" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1520,10 +1575,238 @@
       <c r="D55" s="14"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D56" s="14"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C63" s="7"/>
+      <c r="A56" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" s="5">
+        <v>2025</v>
+      </c>
+      <c r="C56" s="17">
+        <v>4.8300000000000003E-2</v>
+      </c>
+      <c r="D56" s="14">
+        <v>4120333</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B57" s="5">
+        <v>2024</v>
+      </c>
+      <c r="C57" s="17">
+        <v>4.6199999999999998E-2</v>
+      </c>
+      <c r="D57" s="14">
+        <v>4120333</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B58" s="5">
+        <v>2023</v>
+      </c>
+      <c r="C58" s="17">
+        <v>5.9299999999999999E-2</v>
+      </c>
+      <c r="D58" s="14">
+        <v>4120333</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B59" s="5">
+        <v>2022</v>
+      </c>
+      <c r="C59" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="D59" s="14">
+        <v>4120333</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B60" s="5">
+        <v>2021</v>
+      </c>
+      <c r="C60" s="17">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="D60" s="14">
+        <v>4120333</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B61" s="5">
+        <v>2020</v>
+      </c>
+      <c r="C61" s="17">
+        <v>4.3099999999999999E-2</v>
+      </c>
+      <c r="D61" s="14">
+        <v>4120333</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B63" s="5">
+        <v>2025</v>
+      </c>
+      <c r="C63" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="D63" s="14">
+        <v>4123402</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" s="5">
+        <v>2024</v>
+      </c>
+      <c r="C64" s="18">
+        <v>0.04</v>
+      </c>
+      <c r="D64" s="14">
+        <v>4123402</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B65" s="5">
+        <v>2023</v>
+      </c>
+      <c r="C65" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="D65" s="14">
+        <v>4123402</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" s="5">
+        <v>2022</v>
+      </c>
+      <c r="C66" s="18"/>
+      <c r="D66" s="14">
+        <v>4123402</v>
+      </c>
+      <c r="E66" s="10"/>
+    </row>
+    <row r="67" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" s="5">
+        <v>2021</v>
+      </c>
+      <c r="C67" s="18">
+        <v>0.15</v>
+      </c>
+      <c r="D67" s="14">
+        <v>4123402</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" s="5">
+        <v>2021</v>
+      </c>
+      <c r="C68" s="18">
+        <v>0.15</v>
+      </c>
+      <c r="D68" s="14">
+        <v>4123402</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" s="5">
+        <v>2021</v>
+      </c>
+      <c r="C69" s="18">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="D69" s="14">
+        <v>4123402</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" s="5">
+        <v>2020</v>
+      </c>
+      <c r="C70" s="18">
+        <v>4.3099999999999999E-2</v>
+      </c>
+      <c r="D70" s="14">
+        <v>4123402</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>75</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1568,215 +1851,224 @@
     <hyperlink ref="E53" r:id="rId39" display="https://leismunicipais.com.br/a/pr/p/primeiro-de-maio/lei-ordinaria/2021/77/770/lei-ordinaria-n-770-2021-dispoe-sobre-a-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-municipais-de-primeiro-de-maio-e-da-outras-providencias?q=revis%E3o%20geral%20anual%20" xr:uid="{C52DDB23-FB88-489B-BD74-E79A0801ADF5}"/>
     <hyperlink ref="E38" r:id="rId40" xr:uid="{878A7E66-55B4-4DAF-8A75-A1CF624BBEC7}"/>
     <hyperlink ref="E37" r:id="rId41" xr:uid="{47F34AB3-0A0A-412F-8FE1-03EF5CACC9CA}"/>
+    <hyperlink ref="E59" r:id="rId42" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-complementar/2022/59/583/lei-complementar-n-583-2022-dispoe-sobre-aumento-salarial-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=aumento%20salarial" xr:uid="{9456DAAA-0A8A-485D-A402-82BED62E4A97}"/>
+    <hyperlink ref="E56" r:id="rId43" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2025/63/630/lei-ordinaria-n-630-2025-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{64BC75ED-1964-4204-BAFA-49F3A4083336}"/>
+    <hyperlink ref="E57" r:id="rId44" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2024/62/614/lei-ordinaria-n-614-2024-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{0661ED8C-7E04-4235-BDA6-165CAA2FD04B}"/>
+    <hyperlink ref="E58" r:id="rId45" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2023/59/588/lei-ordinaria-n-588-2023-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{4A341ABB-8BE7-4A6E-B4C1-532DBB4378D2}"/>
+    <hyperlink ref="E60" r:id="rId46" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2021/54/534/lei-ordinaria-n-534-2021-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{95B75048-0C9A-47CB-8A73-3D8052953EA1}"/>
+    <hyperlink ref="E61" r:id="rId47" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2020/52/516/lei-ordinaria-n-516-2020-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{46529EB6-AC15-4D01-B558-28DB00531128}"/>
+    <hyperlink ref="E63" r:id="rId48" xr:uid="{EE42FF6B-39FA-43BE-8F7C-A56762A03BE5}"/>
+    <hyperlink ref="E64" r:id="rId49" display="https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2024/232/2320/lei-ordinaria-n-2320-2024-autoriza-revisao-geral-da-remuneracao-e-os-subsidios-dos-servidores-publicos-e-agentes-politicos-dos-poderes-executivo-e-legislativo-do-municipio-nos-termos-do-artigo-7-caput-iv-e-o-do-artigo-39-3-da-constituicao-federal-extensivo-aos-conselheiros-tutelares-e-aos-proventos-dos-inativos-e-pensionistas?q=Revis%C3%A3o+geraL" xr:uid="{4F7B275E-5955-4B1B-94E6-A35B6D80FEE2}"/>
+    <hyperlink ref="E69" r:id="rId50" display="https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2021/218/2180/lei-ordinaria-n-2180-2021-suspende-os-efeitos-da-lei-municipal-n-2147-2021-que-autoriza-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-e-da-outras-providencias?q=Revis%E3o%20geraL" xr:uid="{EB57F7DB-CDEF-4A7C-9E25-23B1204FA785}"/>
+    <hyperlink ref="E70" r:id="rId51" display="https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2020/211/2107/lei-ordinaria-n-2107-2020-autoriza-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-a-aplicacao-do-artigo-7-inciso-iv-e-art-39-3-da-constituicao-federal-a-remuneracao-dos-servidores-publicos-o-reajuste-dos-proventos-dos-inativos-e-pensionistas-a-recomposicao-dos-subsidios-dos-agentes-politicos-e-fixa-os-pisos-nacionais-minimos-para-os-integrantes-do-magisterio-municipal-11739-2008-e-da-outras-providencias?q=Revis%E3o%20geraL" xr:uid="{924B3E23-6A28-4DA7-BF55-853A35BD0084}"/>
+    <hyperlink ref="E67" r:id="rId52" display="https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2021/220/2198/lei-ordinaria-n-2198-2021-autoriza-revisao-geral-da-remuneracao-dos-servidores-publicos-autoriza-a-aplicacao-do-artigo-7-caput-iv-e-o-do-artigo-39-3-da-constituicao-federal-a-remuneracao-dos-servidores-publicos-e-autoriza-o-reajuste-dos-proventos-dos-inativos-e-pensionistas?q=2.198" xr:uid="{D3688214-1F73-4C24-86E5-7E744B395889}"/>
+    <hyperlink ref="E68" r:id="rId53" display="https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2021/220/2197/lei-ordinaria-n-2197-2021-autoriza-revisao-geral-da-remuneracao-dos-servidores-publicos-autoriza-a-aplicacao-do-artigo-7-caput-iv-e-o-do-artigo-39-3-da-constituicao-federal-a-remuneracao-dos-servidores-publicos-e-autoriza-o-reajuste-dos-proventos-dos-inativos-e-pensionistas?q=2.197" xr:uid="{824C9DCD-78D8-43FD-8DB5-0E165BC5D312}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId42"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId54"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD7E18E-7E3E-4609-9E74-70EF657891A1}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B1" s="5">
         <v>2025</v>
       </c>
-      <c r="C1" s="7">
-        <v>4.8300000000000003E-2</v>
+      <c r="C1" s="16">
+        <v>0</v>
       </c>
       <c r="D1" s="14">
-        <v>4120333</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>4109203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B2" s="5">
         <v>2024</v>
       </c>
-      <c r="C2" s="7">
-        <v>4.6199999999999998E-2</v>
+      <c r="C2" s="16">
+        <v>0</v>
       </c>
       <c r="D2" s="14">
-        <v>4120333</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>4109203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B3" s="5">
         <v>2023</v>
       </c>
-      <c r="C3" s="7">
-        <v>5.9299999999999999E-2</v>
+      <c r="C3" s="16">
+        <v>0</v>
       </c>
       <c r="D3" s="14">
-        <v>4120333</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>4109203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B4" s="5">
         <v>2022</v>
       </c>
-      <c r="C4" s="7">
-        <v>0.1</v>
+      <c r="C4" s="16">
+        <v>0</v>
       </c>
       <c r="D4" s="14">
-        <v>4120333</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>4109203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B5" s="5">
         <v>2021</v>
       </c>
-      <c r="C5" s="7">
-        <v>4.5199999999999997E-2</v>
+      <c r="C5" s="16">
+        <v>0</v>
       </c>
       <c r="D5" s="14">
-        <v>4120333</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>4109203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B6" s="5">
         <v>2020</v>
       </c>
-      <c r="C6" s="7">
-        <v>4.3099999999999999E-2</v>
+      <c r="C6" s="16">
+        <v>0</v>
       </c>
       <c r="D6" s="14">
-        <v>4120333</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+        <v>4109203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D7" s="14"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B8" s="5">
         <v>2025</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="16">
         <v>0</v>
       </c>
       <c r="D8" s="14">
-        <v>4109203</v>
+        <v>4120002</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B9" s="5">
         <v>2024</v>
       </c>
       <c r="C9" s="7">
-        <v>0</v>
+        <v>4.6199999999999998E-2</v>
       </c>
       <c r="D9" s="14">
-        <v>4109203</v>
+        <v>4120002</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B10" s="5">
         <v>2023</v>
       </c>
       <c r="C10" s="7">
-        <v>0</v>
+        <v>5.9299999999999999E-2</v>
       </c>
       <c r="D10" s="14">
-        <v>4109203</v>
+        <v>4120002</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B11" s="5">
         <v>2022</v>
       </c>
       <c r="C11" s="7">
-        <v>0</v>
+        <v>0.1016</v>
       </c>
       <c r="D11" s="14">
-        <v>4109203</v>
+        <v>4120002</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B12" s="5">
         <v>2021</v>
       </c>
       <c r="C12" s="7">
-        <v>0</v>
+        <v>4.5199999999999997E-2</v>
       </c>
       <c r="D12" s="14">
-        <v>4109203</v>
+        <v>4120002</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B13" s="5">
         <v>2020</v>
       </c>
       <c r="C13" s="7">
-        <v>0</v>
+        <v>6.5500000000000003E-2</v>
       </c>
       <c r="D13" s="14">
-        <v>4109203</v>
+        <v>4120002</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1784,99 +2076,96 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B15" s="5">
         <v>2025</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="16">
         <v>0</v>
       </c>
       <c r="D15" s="14">
-        <v>4120002</v>
+        <v>4108007</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B16" s="5">
         <v>2024</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="16">
         <v>0</v>
       </c>
       <c r="D16" s="14">
-        <v>4120002</v>
+        <v>4108007</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B17" s="5">
         <v>2023</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="16">
         <v>0</v>
       </c>
       <c r="D17" s="14">
-        <v>4120002</v>
+        <v>4108007</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B18" s="5">
         <v>2022</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="16">
         <v>0</v>
       </c>
       <c r="D18" s="14">
-        <v>4120002</v>
+        <v>4108007</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B19" s="5">
         <v>2021</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="16">
         <v>0</v>
       </c>
       <c r="D19" s="14">
-        <v>4120002</v>
+        <v>4108007</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B20" s="5">
         <v>2020</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="16">
         <v>0</v>
       </c>
       <c r="D20" s="14">
-        <v>4120002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D21" s="14"/>
+        <v>4108007</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B22" s="5">
         <v>2025</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="16">
         <v>0</v>
       </c>
       <c r="D22" s="14">
@@ -1885,12 +2174,12 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B23" s="5">
         <v>2024</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="16">
         <v>0</v>
       </c>
       <c r="D23" s="14">
@@ -1899,12 +2188,12 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B24" s="5">
         <v>2023</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="16">
         <v>0</v>
       </c>
       <c r="D24" s="14">
@@ -1913,12 +2202,12 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B25" s="5">
         <v>2022</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="16">
         <v>0</v>
       </c>
       <c r="D25" s="14">
@@ -1927,12 +2216,12 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B26" s="5">
         <v>2021</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="16">
         <v>0</v>
       </c>
       <c r="D26" s="14">
@@ -1941,26 +2230,28 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B27" s="5">
         <v>2020</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="16">
         <v>0</v>
       </c>
       <c r="D27" s="14">
         <v>4108007</v>
       </c>
     </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" s="15"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-complementar/2022/59/583/lei-complementar-n-583-2022-dispoe-sobre-aumento-salarial-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=aumento%20salarial" xr:uid="{7A2912B1-A033-4B0B-8FE9-0051BC578F1E}"/>
-    <hyperlink ref="E1" r:id="rId2" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2025/63/630/lei-ordinaria-n-630-2025-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{C25B9C11-3CAB-45EA-8DAC-5798EA66F1FB}"/>
-    <hyperlink ref="E2" r:id="rId3" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2024/62/614/lei-ordinaria-n-614-2024-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{180B63DB-B3CA-4BE9-BE93-A756811226FC}"/>
-    <hyperlink ref="E3" r:id="rId4" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2023/59/588/lei-ordinaria-n-588-2023-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{27C5E00F-A21E-4F3D-B440-EEA8732A0606}"/>
-    <hyperlink ref="E5" r:id="rId5" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2021/54/534/lei-ordinaria-n-534-2021-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{A8A960AF-CE07-462C-818F-7309432BE808}"/>
-    <hyperlink ref="E6" r:id="rId6" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2020/52/516/lei-ordinaria-n-516-2020-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{65B1BDEA-E442-424A-AFC9-2BF060B58188}"/>
+    <hyperlink ref="E11" r:id="rId1" display="https://leismunicipais.com.br/a1/pr/p/porecatu/lei-ordinaria/2022/193/1928/lei-ordinaria-n-1928-2022-dispoe-sobre-a-reposicao-salarial-dos-cargos-pertencentes-ao-quadro-proprio-de-servidores-publicos-do-municipio-de-porecatu-inclusive-inativos-e-pensionistas-e-dos-subsidios-dos-secretarios-municipais-prefeito-e-vice-prefeito-e-da-outras-providencias?q=reajuste" xr:uid="{92EE89C2-6E20-497C-9A64-31E1DA7DEEB6}"/>
+    <hyperlink ref="E9" r:id="rId2" display="https://leismunicipais.com.br/a1/pr/p/porecatu/lei-ordinaria/2024/200/1991/lei-ordinaria-n-1991-2024-concede-a-reposicao-de-perdas-salariais-aos-servidores-ativos-e-inativos-e-aos-vereadores-do-poder-legislativo-da-camara-municipal-de-porecatu-e-da-outras-proviencias?q=REPOSI%C7%C3O%20SALARIAL" xr:uid="{F9A76A7A-02CE-4A05-8090-85FBCD779B1E}"/>
+    <hyperlink ref="E10" r:id="rId3" display="https://leismunicipais.com.br/a1/pr/p/porecatu/lei-ordinaria/2023/198/1971/lei-ordinaria-n-1971-2023-dispoe-sobre-a-reposicao-salarial-dos-cargos-pertencentes-ao-quadro-proprio-de-servidores-publicos-do-municipio-de-porecatu-inclusive-inativos-e-pensionistas-e-dos-subsidios-dos-secretarios-municipais-e-da-outras-providencias?q=REPOSI%C7%C3O%20SALARIAL" xr:uid="{DF270D6B-0080-42E7-9C18-644BEEB3D9E0}"/>
+    <hyperlink ref="E12" r:id="rId4" display="https://leismunicipais.com.br/a1/pr/p/porecatu/lei-ordinaria/2021/190/1893/lei-ordinaria-n-1893-2021-dispoe-sobre-a-reposicao-salarial-dos-cargos-pertencentes-ao-quadro-proprio-de-servidores-publicos-do-municipio-de-porecatu-inclusive-inativos-e-pensionistas-e-dos-subsidios-dos-secretarios-municipais-e-da-outras-providencias?q=REPOSI%C7%C3O%20SALARIAL" xr:uid="{419D1B64-7715-4912-9A5A-6F720A207148}"/>
+    <hyperlink ref="E13" r:id="rId5" display="https://leismunicipais.com.br/a1/pr/p/porecatu/lei-ordinaria/2020/186/1857/lei-ordinaria-n-1857-2020-dispoe-sobre-a-reposicao-salarial-dos-cargos-pertencentes-ao-quadro-proprio-de-servidores-publicos-do-municipio-de-porecatu-inclusive-inativos-e-pensionistas-e-dos-subsidios-dos-secretarios-municipais-e-da-outras-providencias?q=REPOSI%C7%C3O%20SALARIAL" xr:uid="{6915330C-711A-4CAB-8DE4-2F8CA66A01E4}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
added   2023  santa fe
</commit_message>
<xml_diff>
--- a/data/dados.xlsx
+++ b/data/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\reajuste\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB2AE3F-94DD-4174-8385-B157466CC0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389DA385-756A-45F1-8B0A-3FB2635211C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{BE2A1F3B-6535-41F1-9783-CEB15E5262F6}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="79">
   <si>
     <t>Cafeara</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>Miraselva</t>
+  </si>
+  <si>
+    <t>https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2023/226/2251/lei-ordinaria-n-2251-2023-autoriza-revisao-geral-da-remuneracao-e-os-subsidios-dos-servidores-publicos-e-agentes-politicos-dos-poderes-executivo-e-legislativo-do-municipio-nos-termos-do-artigo-7-caput-iv-e-o-do-artigo-39-3-da-constituicao-federal-extensivo-aos-conselheiros-tutelares-e-aos-proventos-dos-inativos-e-pensionistas?q=Autoriza%20revis%E3o%20geral%20da%20remunera%E7%E3o</t>
   </si>
 </sst>
 </file>
@@ -730,7 +733,7 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1711,11 +1714,15 @@
       <c r="B65" s="5">
         <v>2023</v>
       </c>
-      <c r="C65" s="7"/>
+      <c r="C65" s="7">
+        <v>0.1</v>
+      </c>
       <c r="D65" s="14">
         <v>4123402</v>
       </c>
-      <c r="E65" s="10"/>
+      <c r="E65" s="10" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="66" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
@@ -1853,9 +1860,10 @@
     <hyperlink ref="E70" r:id="rId51" display="https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2020/211/2107/lei-ordinaria-n-2107-2020-autoriza-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-a-aplicacao-do-artigo-7-inciso-iv-e-art-39-3-da-constituicao-federal-a-remuneracao-dos-servidores-publicos-o-reajuste-dos-proventos-dos-inativos-e-pensionistas-a-recomposicao-dos-subsidios-dos-agentes-politicos-e-fixa-os-pisos-nacionais-minimos-para-os-integrantes-do-magisterio-municipal-11739-2008-e-da-outras-providencias?q=Revis%E3o%20geraL" xr:uid="{924B3E23-6A28-4DA7-BF55-853A35BD0084}"/>
     <hyperlink ref="E67" r:id="rId52" display="https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2021/220/2198/lei-ordinaria-n-2198-2021-autoriza-revisao-geral-da-remuneracao-dos-servidores-publicos-autoriza-a-aplicacao-do-artigo-7-caput-iv-e-o-do-artigo-39-3-da-constituicao-federal-a-remuneracao-dos-servidores-publicos-e-autoriza-o-reajuste-dos-proventos-dos-inativos-e-pensionistas?q=2.198" xr:uid="{D3688214-1F73-4C24-86E5-7E744B395889}"/>
     <hyperlink ref="E68" r:id="rId53" display="https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2021/220/2197/lei-ordinaria-n-2197-2021-autoriza-revisao-geral-da-remuneracao-dos-servidores-publicos-autoriza-a-aplicacao-do-artigo-7-caput-iv-e-o-do-artigo-39-3-da-constituicao-federal-a-remuneracao-dos-servidores-publicos-e-autoriza-o-reajuste-dos-proventos-dos-inativos-e-pensionistas?q=2.197" xr:uid="{824C9DCD-78D8-43FD-8DB5-0E165BC5D312}"/>
+    <hyperlink ref="E65" r:id="rId54" display="https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2023/226/2251/lei-ordinaria-n-2251-2023-autoriza-revisao-geral-da-remuneracao-e-os-subsidios-dos-servidores-publicos-e-agentes-politicos-dos-poderes-executivo-e-legislativo-do-municipio-nos-termos-do-artigo-7-caput-iv-e-o-do-artigo-39-3-da-constituicao-federal-extensivo-aos-conselheiros-tutelares-e-aos-proventos-dos-inativos-e-pensionistas?q=Autoriza%20revis%E3o%20geral%20da%20remunera%E7%E3o" xr:uid="{7E99F84F-40DA-489D-BFB8-FC337539CA92}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId54"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId55"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
ajuste execucao das leis
</commit_message>
<xml_diff>
--- a/data/dados.xlsx
+++ b/data/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\reajuste\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389DA385-756A-45F1-8B0A-3FB2635211C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D015ACB-3A31-456C-A82D-15320DA78358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{BE2A1F3B-6535-41F1-9783-CEB15E5262F6}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="79">
   <si>
     <t>Cafeara</t>
   </si>
@@ -730,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A9F774-A2B7-43E0-89BB-A01627A8B05C}">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1731,18 +1731,22 @@
       <c r="B66" s="5">
         <v>2022</v>
       </c>
-      <c r="C66" s="7"/>
+      <c r="C66" s="7">
+        <v>0.15</v>
+      </c>
       <c r="D66" s="14">
         <v>4123402</v>
       </c>
-      <c r="E66" s="10"/>
+      <c r="E66" s="10" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="67" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B67" s="5">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C67" s="7">
         <v>0.15</v>
@@ -1751,7 +1755,7 @@
         <v>4123402</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="68" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -1762,13 +1766,13 @@
         <v>2021</v>
       </c>
       <c r="C68" s="7">
-        <v>0.15</v>
+        <v>4.5199999999999997E-2</v>
       </c>
       <c r="D68" s="14">
         <v>4123402</v>
       </c>
       <c r="E68" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="69" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -1776,32 +1780,15 @@
         <v>70</v>
       </c>
       <c r="B69" s="5">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C69" s="7">
-        <v>4.5199999999999997E-2</v>
+        <v>4.3099999999999999E-2</v>
       </c>
       <c r="D69" s="14">
         <v>4123402</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B70" s="5">
-        <v>2020</v>
-      </c>
-      <c r="C70" s="7">
-        <v>4.3099999999999999E-2</v>
-      </c>
-      <c r="D70" s="14">
-        <v>4123402</v>
-      </c>
-      <c r="E70" s="10" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1856,10 +1843,10 @@
     <hyperlink ref="E61" r:id="rId47" display="https://leismunicipais.com.br/a2/pr/p/prado-ferreira/lei-ordinaria/2020/52/516/lei-ordinaria-n-516-2020-dispoe-sobre-a-reposicao-de-perdas-salariais-dos-servidores-publicos-do-municipio-de-prado-ferreira-estado-do-parana-e-da-outras-providencias?q=salarial" xr:uid="{46529EB6-AC15-4D01-B558-28DB00531128}"/>
     <hyperlink ref="E63" r:id="rId48" xr:uid="{EE42FF6B-39FA-43BE-8F7C-A56762A03BE5}"/>
     <hyperlink ref="E64" r:id="rId49" display="https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2024/232/2320/lei-ordinaria-n-2320-2024-autoriza-revisao-geral-da-remuneracao-e-os-subsidios-dos-servidores-publicos-e-agentes-politicos-dos-poderes-executivo-e-legislativo-do-municipio-nos-termos-do-artigo-7-caput-iv-e-o-do-artigo-39-3-da-constituicao-federal-extensivo-aos-conselheiros-tutelares-e-aos-proventos-dos-inativos-e-pensionistas?q=Revis%C3%A3o+geraL" xr:uid="{4F7B275E-5955-4B1B-94E6-A35B6D80FEE2}"/>
-    <hyperlink ref="E69" r:id="rId50" display="https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2021/218/2180/lei-ordinaria-n-2180-2021-suspende-os-efeitos-da-lei-municipal-n-2147-2021-que-autoriza-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-e-da-outras-providencias?q=Revis%E3o%20geraL" xr:uid="{EB57F7DB-CDEF-4A7C-9E25-23B1204FA785}"/>
-    <hyperlink ref="E70" r:id="rId51" display="https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2020/211/2107/lei-ordinaria-n-2107-2020-autoriza-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-a-aplicacao-do-artigo-7-inciso-iv-e-art-39-3-da-constituicao-federal-a-remuneracao-dos-servidores-publicos-o-reajuste-dos-proventos-dos-inativos-e-pensionistas-a-recomposicao-dos-subsidios-dos-agentes-politicos-e-fixa-os-pisos-nacionais-minimos-para-os-integrantes-do-magisterio-municipal-11739-2008-e-da-outras-providencias?q=Revis%E3o%20geraL" xr:uid="{924B3E23-6A28-4DA7-BF55-853A35BD0084}"/>
-    <hyperlink ref="E67" r:id="rId52" display="https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2021/220/2198/lei-ordinaria-n-2198-2021-autoriza-revisao-geral-da-remuneracao-dos-servidores-publicos-autoriza-a-aplicacao-do-artigo-7-caput-iv-e-o-do-artigo-39-3-da-constituicao-federal-a-remuneracao-dos-servidores-publicos-e-autoriza-o-reajuste-dos-proventos-dos-inativos-e-pensionistas?q=2.198" xr:uid="{D3688214-1F73-4C24-86E5-7E744B395889}"/>
-    <hyperlink ref="E68" r:id="rId53" display="https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2021/220/2197/lei-ordinaria-n-2197-2021-autoriza-revisao-geral-da-remuneracao-dos-servidores-publicos-autoriza-a-aplicacao-do-artigo-7-caput-iv-e-o-do-artigo-39-3-da-constituicao-federal-a-remuneracao-dos-servidores-publicos-e-autoriza-o-reajuste-dos-proventos-dos-inativos-e-pensionistas?q=2.197" xr:uid="{824C9DCD-78D8-43FD-8DB5-0E165BC5D312}"/>
+    <hyperlink ref="E68" r:id="rId50" display="https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2021/218/2180/lei-ordinaria-n-2180-2021-suspende-os-efeitos-da-lei-municipal-n-2147-2021-que-autoriza-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-e-da-outras-providencias?q=Revis%E3o%20geraL" xr:uid="{EB57F7DB-CDEF-4A7C-9E25-23B1204FA785}"/>
+    <hyperlink ref="E69" r:id="rId51" display="https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2020/211/2107/lei-ordinaria-n-2107-2020-autoriza-revisao-geral-anual-da-remuneracao-dos-servidores-publicos-a-aplicacao-do-artigo-7-inciso-iv-e-art-39-3-da-constituicao-federal-a-remuneracao-dos-servidores-publicos-o-reajuste-dos-proventos-dos-inativos-e-pensionistas-a-recomposicao-dos-subsidios-dos-agentes-politicos-e-fixa-os-pisos-nacionais-minimos-para-os-integrantes-do-magisterio-municipal-11739-2008-e-da-outras-providencias?q=Revis%E3o%20geraL" xr:uid="{924B3E23-6A28-4DA7-BF55-853A35BD0084}"/>
+    <hyperlink ref="E66" r:id="rId52" display="https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2021/220/2198/lei-ordinaria-n-2198-2021-autoriza-revisao-geral-da-remuneracao-dos-servidores-publicos-autoriza-a-aplicacao-do-artigo-7-caput-iv-e-o-do-artigo-39-3-da-constituicao-federal-a-remuneracao-dos-servidores-publicos-e-autoriza-o-reajuste-dos-proventos-dos-inativos-e-pensionistas?q=2.198" xr:uid="{D3688214-1F73-4C24-86E5-7E744B395889}"/>
+    <hyperlink ref="E67" r:id="rId53" display="https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2021/220/2197/lei-ordinaria-n-2197-2021-autoriza-revisao-geral-da-remuneracao-dos-servidores-publicos-autoriza-a-aplicacao-do-artigo-7-caput-iv-e-o-do-artigo-39-3-da-constituicao-federal-a-remuneracao-dos-servidores-publicos-e-autoriza-o-reajuste-dos-proventos-dos-inativos-e-pensionistas?q=2.197" xr:uid="{824C9DCD-78D8-43FD-8DB5-0E165BC5D312}"/>
     <hyperlink ref="E65" r:id="rId54" display="https://leismunicipais.com.br/a/pr/s/santa-fe/lei-ordinaria/2023/226/2251/lei-ordinaria-n-2251-2023-autoriza-revisao-geral-da-remuneracao-e-os-subsidios-dos-servidores-publicos-e-agentes-politicos-dos-poderes-executivo-e-legislativo-do-municipio-nos-termos-do-artigo-7-caput-iv-e-o-do-artigo-39-3-da-constituicao-federal-extensivo-aos-conselheiros-tutelares-e-aos-proventos-dos-inativos-e-pensionistas?q=Autoriza%20revis%E3o%20geral%20da%20remunera%E7%E3o" xr:uid="{7E99F84F-40DA-489D-BFB8-FC337539CA92}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>